<commit_message>
Mainly just adding burndown chart
Added current sprint and total tasks, to help with the burndown chart
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\QUT\Year 2\Sem 2\IFB299\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23310" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23310" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="89">
   <si>
     <t>User story: Database</t>
   </si>
@@ -275,6 +275,18 @@
   </si>
   <si>
     <t>Maybe display the information in a textbox, rather than just plain html</t>
+  </si>
+  <si>
+    <t>Total Tasks</t>
+  </si>
+  <si>
+    <t>Current Velocity</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>Sprint Tasks</t>
   </si>
 </sst>
 </file>
@@ -348,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -456,11 +468,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -470,38 +491,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,7 +510,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -522,10 +554,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -533,143 +565,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1086,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1099,387 +1009,404 @@
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="94.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7" t="s">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="J2" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32">
         <v>6</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>6.1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="19">
         <v>6085</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="8">
+      <c r="J3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
+      <c r="B4" s="7">
         <v>6.2</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>42378</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="8">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="33"/>
+      <c r="B5" s="7">
         <v>6.3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
         <v>0.5</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>42378</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="8">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="33"/>
+      <c r="B6" s="7">
         <v>6.4</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
         <v>0.5</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>42378</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="8">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="33"/>
+      <c r="B7" s="7">
         <v>6.5</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>0.5</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>0.5</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="19">
         <v>6085</v>
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="7">
         <v>6.6</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>36</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>25</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="19">
         <v>6085</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="31"/>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
-        <v>1</v>
-      </c>
-      <c r="B12" s="24">
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="31">
+        <v>1</v>
+      </c>
+      <c r="B12" s="16">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="24">
-        <v>1</v>
-      </c>
-      <c r="E12" s="23">
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15">
         <v>5</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="19">
         <v>6085</v>
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="24">
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="31"/>
+      <c r="B13" s="16">
         <v>1.2</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="16">
         <v>2</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>42409</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="24">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="31"/>
+      <c r="B14" s="16">
         <v>1.3</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="25">
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
+      <c r="B15" s="37">
         <v>1.4</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="25">
-        <v>1</v>
-      </c>
-      <c r="E15" s="26">
-        <v>1</v>
-      </c>
-      <c r="F15" s="26" t="s">
+      <c r="D15" s="37">
+        <v>1</v>
+      </c>
+      <c r="E15" s="35">
+        <v>1</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="36">
         <v>42378</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="29" t="s">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="23">
+      <c r="A17" s="31"/>
+      <c r="B17" s="15">
         <v>1.5</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="23">
-        <v>1</v>
-      </c>
-      <c r="E17" s="23">
-        <v>1</v>
-      </c>
-      <c r="F17" s="23" t="s">
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="19">
         <v>6085</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="29"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H20" s="5" t="s">
@@ -1487,25 +1414,25 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="32">
         <v>11</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="9">
         <v>11.1</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="9">
         <v>0.5</v>
       </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>42378</v>
       </c>
       <c r="H21" s="5" t="s">
@@ -1513,23 +1440,23 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="13">
+      <c r="A22" s="33"/>
+      <c r="B22" s="9">
         <v>11.2</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="9">
         <v>0.5</v>
       </c>
-      <c r="E22" s="8">
-        <v>1</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="19">
         <v>6085</v>
       </c>
       <c r="H22" s="5" t="s">
@@ -1537,51 +1464,51 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="17"/>
+      <c r="H25" s="29"/>
     </row>
     <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H26" s="5" t="s">
@@ -1589,25 +1516,25 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
+      <c r="A27" s="31">
         <v>12</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="9">
         <v>12.1</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="9">
         <v>3</v>
       </c>
-      <c r="E27" s="8">
-        <v>1</v>
-      </c>
-      <c r="F27" s="18" t="s">
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="8">
         <v>42378</v>
       </c>
       <c r="H27" s="5" t="s">
@@ -1615,45 +1542,45 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="13">
+      <c r="A28" s="31"/>
+      <c r="B28" s="9">
         <v>12.2</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="13">
-        <v>1</v>
-      </c>
-      <c r="E28" s="8">
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7">
         <v>0.5</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="8">
         <v>42378</v>
       </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="13">
+      <c r="A29" s="31"/>
+      <c r="B29" s="9">
         <v>12.3</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="9">
         <v>2</v>
       </c>
-      <c r="E29" s="8">
-        <v>1</v>
-      </c>
-      <c r="F29" s="8" t="s">
+      <c r="E29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="8">
         <v>42378</v>
       </c>
       <c r="H29" s="5"/>
@@ -1664,41 +1591,41 @@
       <c r="D30" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7" t="s">
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H33" s="5" t="s">
@@ -1706,67 +1633,67 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="14"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="10"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1787,13 +1714,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="G15:G16"/>
@@ -1805,6 +1725,13 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="D15:D16"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A25:E25"/>
   </mergeCells>
@@ -1819,10 +1746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1835,372 +1762,390 @@
     <col min="8" max="8" width="93.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="36" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="15" t="s">
+      <c r="G1" s="42"/>
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
+      <c r="J2" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31">
         <v>21</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>21.1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>5</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>42378</v>
       </c>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="8">
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>24</v>
+      </c>
+      <c r="L3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31"/>
+      <c r="B4" s="7">
         <v>21.2</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>42378</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="8">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
+      <c r="B5" s="7">
         <v>21.3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="8">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="31"/>
+      <c r="B6" s="7">
         <v>21.4</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
-      <c r="B7" s="8">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
+      <c r="B7" s="7">
         <v>21.5</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="7">
         <v>21.6</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="8">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
+      <c r="B9" s="7">
         <v>21.7</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="14"/>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="8">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="31"/>
+      <c r="B10" s="7">
         <v>21.8</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>42378</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="8">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="31"/>
+      <c r="B11" s="7">
         <v>21.9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>10</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="36" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="15" t="s">
+      <c r="G13" s="42"/>
+      <c r="H13" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="32">
         <v>20</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>20.100000000000001</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>0.5</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="33"/>
+      <c r="B16" s="7">
         <v>20.2</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0.5</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="8">
+      <c r="A17" s="33"/>
+      <c r="B17" s="7">
         <v>20.3</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>0.5</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="8">
+      <c r="A18" s="34"/>
+      <c r="B18" s="7">
         <v>20.399999999999999</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>0.5</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="36" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="15" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H21" s="5" t="s">
@@ -2208,77 +2153,77 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20">
+      <c r="A22" s="31">
         <v>5</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="23">
         <v>0.5</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="40" t="s">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="24" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="8">
+      <c r="A23" s="31"/>
+      <c r="B23" s="7">
         <v>5.2</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="23">
         <v>0.5</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="36" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="15" t="s">
+      <c r="G25" s="42"/>
+      <c r="H25" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H26" s="5" t="s">
@@ -2286,101 +2231,101 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19">
+      <c r="A27" s="13">
         <v>8</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="7">
         <v>8.1</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="8">
-        <v>1</v>
-      </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="8">
+      <c r="A28" s="13"/>
+      <c r="B28" s="7">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="8">
-        <v>1</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="8">
+      <c r="A29" s="13"/>
+      <c r="B29" s="7">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="8">
-        <v>1</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="40" t="s">
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="8">
+      <c r="A30" s="13"/>
+      <c r="B30" s="7">
         <v>8.4</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="8">
-        <v>1</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="8">
+      <c r="A31" s="13"/>
+      <c r="B31" s="7">
         <v>8.5</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <v>0.5</v>
       </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="14"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -2390,41 +2335,41 @@
       <c r="H33" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="36" t="s">
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G35" s="37"/>
-      <c r="H35" s="15" t="s">
+      <c r="G35" s="42"/>
+      <c r="H35" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H36" s="5" t="s">
@@ -2432,103 +2377,103 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19">
+      <c r="A37" s="13">
         <v>4</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="7">
         <v>5</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="43" t="s">
+      <c r="E37" s="10"/>
+      <c r="F37" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="14"/>
+      <c r="G37" s="10"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
-      <c r="B38" s="8">
+      <c r="A38" s="13"/>
+      <c r="B38" s="7">
         <v>4.2</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="7">
         <v>5</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="43" t="s">
+      <c r="E38" s="10"/>
+      <c r="F38" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="14"/>
+      <c r="G38" s="10"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="19"/>
-      <c r="B39" s="8">
+      <c r="A39" s="13"/>
+      <c r="B39" s="7">
         <v>4.3</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="8">
-        <v>1</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
+      <c r="D39" s="7">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="19"/>
-      <c r="B40" s="8">
+      <c r="A40" s="13"/>
+      <c r="B40" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="8">
-        <v>1</v>
-      </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="40" t="s">
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="8">
+      <c r="A41" s="13"/>
+      <c r="B41" s="7">
         <v>4.5</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19"/>
-      <c r="B42" s="8">
+      <c r="A42" s="13"/>
+      <c r="B42" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="14"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -2539,19 +2484,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 F13 H13">
     <cfRule type="notContainsBlanks" dxfId="8" priority="12">

</xml_diff>

<commit_message>
Moved events attending page
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -788,18 +788,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -822,15 +822,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -839,11 +842,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1682,9 +1682,9 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>6.2</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>6.3</v>
       </c>
@@ -1815,7 +1815,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>6.4</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>6.5</v>
       </c>
@@ -1863,7 +1863,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="5">
         <v>6.6</v>
       </c>
@@ -1894,17 +1894,17 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="47"/>
       <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="52" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="47"/>
@@ -1938,7 +1938,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="51">
+      <c r="A12" s="49">
         <v>1</v>
       </c>
       <c r="B12" s="17">
@@ -1963,7 +1963,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="17">
         <v>1.2</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="17">
         <v>1.3</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="55">
         <v>1.4</v>
       </c>
@@ -2017,27 +2017,27 @@
       <c r="F15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="53">
         <v>42378</v>
       </c>
       <c r="H15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
       <c r="H16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="16">
         <v>1.5</v>
       </c>
@@ -2071,9 +2071,9 @@
       <c r="A19" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="47"/>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -2112,7 +2112,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51">
+      <c r="A21" s="49">
         <v>11</v>
       </c>
       <c r="B21" s="22">
@@ -2139,7 +2139,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="22">
         <v>11.2</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2186,9 +2186,9 @@
       <c r="A25" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="1" t="s">
         <v>42</v>
@@ -2227,7 +2227,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>12</v>
       </c>
       <c r="B27" s="22">
@@ -2254,7 +2254,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="22">
         <v>12.2</v>
       </c>
@@ -2277,7 +2277,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="22">
         <v>12.3</v>
       </c>
@@ -2320,9 +2320,9 @@
       <c r="A32" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="47"/>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -2361,7 +2361,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="51"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2372,7 +2372,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="52"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2383,7 +2383,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="52"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2394,7 +2394,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="52"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2405,7 +2405,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="52"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2416,7 +2416,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2427,7 +2427,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -10123,15 +10123,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G15:G16"/>
@@ -10143,6 +10134,15 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 A1 F10:G10 A10 F19:G19 A19 F25:G25 A25 F32:G32 A32">
     <cfRule type="notContainsBlanks" dxfId="37" priority="1">
@@ -10179,9 +10179,9 @@
       <c r="A1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="58" t="s">
         <v>1</v>
@@ -10227,7 +10227,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>21</v>
       </c>
       <c r="B3" s="5">
@@ -10260,7 +10260,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>21.2</v>
       </c>
@@ -10284,7 +10284,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>21.3</v>
       </c>
@@ -10308,7 +10308,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>21.4</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>21.5</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="5">
         <v>21.6</v>
       </c>
@@ -10376,7 +10376,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="5">
         <v>21.7</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="5">
         <v>21.8</v>
       </c>
@@ -10422,7 +10422,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="5">
         <v>21.9</v>
       </c>
@@ -10458,9 +10458,9 @@
       <c r="A13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="47"/>
       <c r="F13" s="58" t="s">
         <v>42</v>
@@ -10497,7 +10497,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="51">
+      <c r="A15" s="49">
         <v>20</v>
       </c>
       <c r="B15" s="5">
@@ -10521,7 +10521,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="5">
         <v>20.2</v>
       </c>
@@ -10543,7 +10543,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="5">
         <v>20.3</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -10600,9 +10600,9 @@
       <c r="A20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="47"/>
       <c r="F20" s="58" t="s">
         <v>49</v>
@@ -10639,7 +10639,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51">
+      <c r="A22" s="49">
         <v>5</v>
       </c>
       <c r="B22" s="5">
@@ -10661,7 +10661,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5">
         <v>5.2</v>
       </c>
@@ -10690,9 +10690,9 @@
       <c r="A25" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="58" t="s">
         <v>40</v>
@@ -10729,7 +10729,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>8</v>
       </c>
       <c r="B27" s="5">
@@ -10854,9 +10854,9 @@
       <c r="A33" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="47"/>
       <c r="F33" s="58" t="s">
         <v>70</v>
@@ -10893,7 +10893,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51">
+      <c r="A35" s="49">
         <v>4</v>
       </c>
       <c r="B35" s="5">
@@ -18705,7 +18705,7 @@
   <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136:B142"/>
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18725,9 +18725,9 @@
       <c r="A1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
@@ -18770,7 +18770,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="69">
+      <c r="A3" s="62">
         <v>22</v>
       </c>
       <c r="B3" s="31">
@@ -18800,7 +18800,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="69"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="31">
         <v>22.2</v>
       </c>
@@ -18822,7 +18822,7 @@
       <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="69"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="31">
         <v>22.3</v>
       </c>
@@ -18847,9 +18847,9 @@
       <c r="A7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="47"/>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -18886,7 +18886,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="69">
+      <c r="A9" s="62">
         <v>33</v>
       </c>
       <c r="B9" s="31">
@@ -18904,7 +18904,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="33">
         <v>33.200000000000003</v>
       </c>
@@ -18920,7 +18920,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="31">
         <v>33.299999999999997</v>
       </c>
@@ -18936,7 +18936,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="31">
         <v>33.4</v>
       </c>
@@ -18952,7 +18952,7 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="31">
         <v>33.5</v>
       </c>
@@ -18971,10 +18971,10 @@
       <c r="A15" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19164,7 +19164,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="62">
+      <c r="A27" s="67">
         <v>35</v>
       </c>
       <c r="B27" s="5">
@@ -19182,7 +19182,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="67"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="31">
         <v>35.200000000000003</v>
       </c>
@@ -19198,7 +19198,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="5">
         <v>35.299999999999997</v>
       </c>
@@ -19214,7 +19214,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="67"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="31">
         <v>35.4</v>
       </c>
@@ -19230,7 +19230,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="67"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="5">
         <v>35.5</v>
       </c>
@@ -19246,7 +19246,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="67"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="31">
         <v>35.6</v>
       </c>
@@ -19262,7 +19262,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="67"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -19278,7 +19278,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="68"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="5">
         <v>35.799999999999997</v>
       </c>
@@ -19336,7 +19336,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="51">
+      <c r="A38" s="49">
         <v>40</v>
       </c>
       <c r="B38" s="5">
@@ -19508,7 +19508,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="51">
+      <c r="A49" s="49">
         <v>23</v>
       </c>
       <c r="B49" s="5">
@@ -19530,7 +19530,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="52"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="5">
         <v>23.2</v>
       </c>
@@ -19550,7 +19550,7 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="52"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="5">
         <v>23.3</v>
       </c>
@@ -19570,7 +19570,7 @@
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="52"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="5">
         <v>23.4</v>
       </c>
@@ -19590,7 +19590,7 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="52"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="5">
         <v>23.5</v>
       </c>
@@ -19610,7 +19610,7 @@
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="52"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="5">
         <v>23.6</v>
       </c>
@@ -19630,7 +19630,7 @@
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="52"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="5">
         <v>23.7</v>
       </c>
@@ -19650,7 +19650,7 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="50"/>
+      <c r="A56" s="51"/>
       <c r="B56" s="5">
         <v>23.8</v>
       </c>
@@ -19712,7 +19712,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="51">
+      <c r="A60" s="49">
         <v>3</v>
       </c>
       <c r="B60" s="5">
@@ -19730,7 +19730,7 @@
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="5">
         <v>3.2</v>
       </c>
@@ -19746,7 +19746,7 @@
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="5">
         <v>3.3</v>
       </c>
@@ -19762,7 +19762,7 @@
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="5">
         <v>3.4</v>
       </c>
@@ -19778,7 +19778,7 @@
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
+      <c r="A64" s="50"/>
       <c r="B64" s="5">
         <v>3.5</v>
       </c>
@@ -19794,7 +19794,7 @@
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
+      <c r="A65" s="50"/>
       <c r="B65" s="5">
         <v>3.6</v>
       </c>
@@ -19810,7 +19810,7 @@
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="50"/>
+      <c r="A66" s="51"/>
       <c r="B66" s="5">
         <v>3.7</v>
       </c>
@@ -19868,7 +19868,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="51">
+      <c r="A70" s="49">
         <v>41</v>
       </c>
       <c r="B70" s="5">
@@ -19888,7 +19888,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="52"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="5">
         <v>41.2</v>
       </c>
@@ -19906,7 +19906,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="52"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="5">
         <v>41.3</v>
       </c>
@@ -19924,7 +19924,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="52"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="5">
         <v>41.4</v>
       </c>
@@ -19942,7 +19942,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="52"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="5">
         <v>41.5</v>
       </c>
@@ -19960,7 +19960,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
+      <c r="A75" s="50"/>
       <c r="B75" s="5">
         <v>41.6</v>
       </c>
@@ -19978,7 +19978,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="50"/>
+      <c r="A76" s="51"/>
       <c r="B76" s="5">
         <v>41.7</v>
       </c>
@@ -20038,7 +20038,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="51">
+      <c r="A80" s="49">
         <v>25</v>
       </c>
       <c r="B80" s="5">
@@ -20060,7 +20060,7 @@
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="52"/>
+      <c r="A81" s="50"/>
       <c r="B81" s="5">
         <v>25.2</v>
       </c>
@@ -20080,7 +20080,7 @@
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="52"/>
+      <c r="A82" s="50"/>
       <c r="B82" s="5">
         <v>25.3</v>
       </c>
@@ -20100,7 +20100,7 @@
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="52"/>
+      <c r="A83" s="50"/>
       <c r="B83" s="5">
         <v>25.4</v>
       </c>
@@ -20120,7 +20120,7 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="52"/>
+      <c r="A84" s="50"/>
       <c r="B84" s="5">
         <v>25.5</v>
       </c>
@@ -20140,7 +20140,7 @@
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="52"/>
+      <c r="A85" s="50"/>
       <c r="B85" s="5">
         <v>25.6</v>
       </c>
@@ -20160,7 +20160,7 @@
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="52"/>
+      <c r="A86" s="50"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -20170,7 +20170,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="50"/>
+      <c r="A87" s="51"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -20222,7 +20222,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="51">
+      <c r="A91" s="49">
         <v>26</v>
       </c>
       <c r="B91" s="39">
@@ -20244,7 +20244,7 @@
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="52"/>
+      <c r="A92" s="50"/>
       <c r="B92" s="39">
         <v>26.2</v>
       </c>
@@ -20264,7 +20264,7 @@
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="52"/>
+      <c r="A93" s="50"/>
       <c r="B93" s="39">
         <v>26.3</v>
       </c>
@@ -20284,7 +20284,7 @@
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="52"/>
+      <c r="A94" s="50"/>
       <c r="B94" s="39">
         <v>26.4</v>
       </c>
@@ -20304,7 +20304,7 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="52"/>
+      <c r="A95" s="50"/>
       <c r="B95" s="39">
         <v>26.5</v>
       </c>
@@ -20324,7 +20324,7 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="52"/>
+      <c r="A96" s="50"/>
       <c r="B96" s="39">
         <v>26.6</v>
       </c>
@@ -20344,7 +20344,7 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
+      <c r="A97" s="50"/>
       <c r="B97" s="39">
         <v>26.7</v>
       </c>
@@ -20364,7 +20364,7 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="52"/>
+      <c r="A98" s="50"/>
       <c r="B98" s="39">
         <v>26.8</v>
       </c>
@@ -20384,7 +20384,7 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="50"/>
+      <c r="A99" s="51"/>
       <c r="B99" s="39">
         <v>26.9</v>
       </c>
@@ -20446,7 +20446,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="51">
+      <c r="A103" s="49">
         <v>27</v>
       </c>
       <c r="B103" s="5">
@@ -20468,7 +20468,7 @@
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="52"/>
+      <c r="A104" s="50"/>
       <c r="B104" s="5">
         <v>27.2</v>
       </c>
@@ -20488,7 +20488,7 @@
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="52"/>
+      <c r="A105" s="50"/>
       <c r="B105" s="5">
         <v>27.3</v>
       </c>
@@ -20508,7 +20508,7 @@
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="52"/>
+      <c r="A106" s="50"/>
       <c r="B106" s="5">
         <v>27.4</v>
       </c>
@@ -20528,7 +20528,7 @@
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="52"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="5">
         <v>27.5</v>
       </c>
@@ -20548,7 +20548,7 @@
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="52"/>
+      <c r="A108" s="50"/>
       <c r="B108" s="5">
         <v>27.6</v>
       </c>
@@ -20568,7 +20568,7 @@
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="50"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="5">
         <v>27.7</v>
       </c>
@@ -20630,7 +20630,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="62">
+      <c r="A113" s="67">
         <v>4</v>
       </c>
       <c r="B113" s="31">
@@ -20650,7 +20650,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="63"/>
+      <c r="A114" s="70"/>
       <c r="B114" s="31">
         <v>4.2</v>
       </c>
@@ -20668,7 +20668,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="63"/>
+      <c r="A115" s="70"/>
       <c r="B115" s="31">
         <v>4.3</v>
       </c>
@@ -20686,7 +20686,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="63"/>
+      <c r="A116" s="70"/>
       <c r="B116" s="31">
         <v>4.4000000000000004</v>
       </c>
@@ -20704,7 +20704,7 @@
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="63"/>
+      <c r="A117" s="70"/>
       <c r="B117" s="31">
         <v>4.5</v>
       </c>
@@ -20722,7 +20722,7 @@
       <c r="H117" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="63"/>
+      <c r="A118" s="70"/>
       <c r="B118" s="31">
         <v>4.5999999999999996</v>
       </c>
@@ -20740,7 +20740,7 @@
       <c r="H118" s="3"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="63"/>
+      <c r="A119" s="70"/>
       <c r="B119" s="31">
         <v>4.7</v>
       </c>
@@ -20758,7 +20758,7 @@
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="63"/>
+      <c r="A120" s="70"/>
       <c r="B120" s="31">
         <v>4.8</v>
       </c>
@@ -20776,7 +20776,7 @@
       <c r="H120" s="3"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="63"/>
+      <c r="A121" s="70"/>
       <c r="B121" s="31">
         <v>4.9000000000000004</v>
       </c>
@@ -20794,7 +20794,7 @@
       <c r="H121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="64"/>
+      <c r="A122" s="71"/>
       <c r="B122" s="31">
         <v>5</v>
       </c>
@@ -20854,7 +20854,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="51">
+      <c r="A126" s="49">
         <v>30</v>
       </c>
       <c r="B126" s="5">
@@ -20874,7 +20874,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="52"/>
+      <c r="A127" s="50"/>
       <c r="B127" s="5">
         <v>27.2</v>
       </c>
@@ -20892,7 +20892,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="52"/>
+      <c r="A128" s="50"/>
       <c r="B128" s="5">
         <v>27.3</v>
       </c>
@@ -20910,7 +20910,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="52"/>
+      <c r="A129" s="50"/>
       <c r="B129" s="5">
         <v>27.4</v>
       </c>
@@ -20928,7 +20928,7 @@
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="52"/>
+      <c r="A130" s="50"/>
       <c r="B130" s="5">
         <v>27.5</v>
       </c>
@@ -20946,7 +20946,7 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="52"/>
+      <c r="A131" s="50"/>
       <c r="B131" s="5">
         <v>27.6</v>
       </c>
@@ -20964,7 +20964,7 @@
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="50"/>
+      <c r="A132" s="51"/>
       <c r="B132" s="5">
         <v>27.7</v>
       </c>
@@ -21024,7 +21024,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="51">
+      <c r="A136" s="49">
         <v>32</v>
       </c>
       <c r="B136" s="5">
@@ -21046,7 +21046,7 @@
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="52"/>
+      <c r="A137" s="50"/>
       <c r="B137" s="5">
         <v>32.200000000000003</v>
       </c>
@@ -21066,7 +21066,7 @@
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="52"/>
+      <c r="A138" s="50"/>
       <c r="B138" s="5">
         <v>32.299999999999997</v>
       </c>
@@ -21086,7 +21086,7 @@
       <c r="H138" s="3"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="52"/>
+      <c r="A139" s="50"/>
       <c r="B139" s="5">
         <v>32.4</v>
       </c>
@@ -21106,7 +21106,7 @@
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="52"/>
+      <c r="A140" s="50"/>
       <c r="B140" s="5">
         <v>32.5</v>
       </c>
@@ -21126,7 +21126,7 @@
       <c r="H140" s="3"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="52"/>
+      <c r="A141" s="50"/>
       <c r="B141" s="5">
         <v>32.6</v>
       </c>
@@ -21146,7 +21146,7 @@
       <c r="H141" s="3"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="50"/>
+      <c r="A142" s="51"/>
       <c r="B142" s="5">
         <v>32.700000000000003</v>
       </c>
@@ -21167,6 +21167,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="A80:A87"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="G134:H134"/>
     <mergeCell ref="A136:A142"/>
@@ -21183,32 +21209,6 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="G36:H36"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="A80:A87"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:A122"/>
   </mergeCells>
   <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="27" priority="23">

</xml_diff>

<commit_message>
Revert "Moved events attending page"
This reverts commit bb55ff27aa3785a8a574227069e00a954d148f4c.
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -788,18 +788,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -822,18 +822,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -842,8 +839,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1682,9 +1682,9 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49">
+      <c r="A3" s="51">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="50"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="5">
         <v>6.2</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="5">
         <v>6.3</v>
       </c>
@@ -1815,7 +1815,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="5">
         <v>6.4</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="5">
         <v>6.5</v>
       </c>
@@ -1863,7 +1863,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="5">
         <v>6.6</v>
       </c>
@@ -1894,17 +1894,17 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="47"/>
       <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="48" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="47"/>
@@ -1938,7 +1938,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49">
+      <c r="A12" s="51">
         <v>1</v>
       </c>
       <c r="B12" s="17">
@@ -1963,7 +1963,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="50"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="17">
         <v>1.2</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="50"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="17">
         <v>1.3</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="50"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="55">
         <v>1.4</v>
       </c>
@@ -2017,27 +2017,27 @@
       <c r="F15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="49">
         <v>42378</v>
       </c>
       <c r="H15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
       <c r="H16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="16">
         <v>1.5</v>
       </c>
@@ -2071,9 +2071,9 @@
       <c r="A19" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="47"/>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -2112,7 +2112,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49">
+      <c r="A21" s="51">
         <v>11</v>
       </c>
       <c r="B21" s="22">
@@ -2139,7 +2139,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="22">
         <v>11.2</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2186,9 +2186,9 @@
       <c r="A25" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="47"/>
       <c r="F25" s="1" t="s">
         <v>42</v>
@@ -2227,7 +2227,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49">
+      <c r="A27" s="51">
         <v>12</v>
       </c>
       <c r="B27" s="22">
@@ -2254,7 +2254,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="22">
         <v>12.2</v>
       </c>
@@ -2277,7 +2277,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="22">
         <v>12.3</v>
       </c>
@@ -2320,9 +2320,9 @@
       <c r="A32" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
       <c r="E32" s="47"/>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -2361,7 +2361,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="49"/>
+      <c r="A34" s="51"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2372,7 +2372,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="50"/>
+      <c r="A35" s="52"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2383,7 +2383,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="50"/>
+      <c r="A36" s="52"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2394,7 +2394,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="50"/>
+      <c r="A37" s="52"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2405,7 +2405,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="50"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2416,7 +2416,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="50"/>
+      <c r="A39" s="52"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2427,7 +2427,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="51"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -10123,6 +10123,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G15:G16"/>
@@ -10134,15 +10143,6 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 A1 F10:G10 A10 F19:G19 A19 F25:G25 A25 F32:G32 A32">
     <cfRule type="notContainsBlanks" dxfId="37" priority="1">
@@ -10179,9 +10179,9 @@
       <c r="A1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="47"/>
       <c r="F1" s="58" t="s">
         <v>1</v>
@@ -10227,7 +10227,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49">
+      <c r="A3" s="51">
         <v>21</v>
       </c>
       <c r="B3" s="5">
@@ -10260,7 +10260,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="50"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="5">
         <v>21.2</v>
       </c>
@@ -10284,7 +10284,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="5">
         <v>21.3</v>
       </c>
@@ -10308,7 +10308,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="5">
         <v>21.4</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="5">
         <v>21.5</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="5">
         <v>21.6</v>
       </c>
@@ -10376,7 +10376,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="50"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="5">
         <v>21.7</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="50"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="5">
         <v>21.8</v>
       </c>
@@ -10422,7 +10422,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="5">
         <v>21.9</v>
       </c>
@@ -10458,9 +10458,9 @@
       <c r="A13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="47"/>
       <c r="F13" s="58" t="s">
         <v>42</v>
@@ -10497,7 +10497,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49">
+      <c r="A15" s="51">
         <v>20</v>
       </c>
       <c r="B15" s="5">
@@ -10521,7 +10521,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="50"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="5">
         <v>20.2</v>
       </c>
@@ -10543,7 +10543,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="5">
         <v>20.3</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="51"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -10600,9 +10600,9 @@
       <c r="A20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="47"/>
       <c r="F20" s="58" t="s">
         <v>49</v>
@@ -10639,7 +10639,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49">
+      <c r="A22" s="51">
         <v>5</v>
       </c>
       <c r="B22" s="5">
@@ -10661,7 +10661,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="5">
         <v>5.2</v>
       </c>
@@ -10690,9 +10690,9 @@
       <c r="A25" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="47"/>
       <c r="F25" s="58" t="s">
         <v>40</v>
@@ -10729,7 +10729,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49">
+      <c r="A27" s="51">
         <v>8</v>
       </c>
       <c r="B27" s="5">
@@ -10854,9 +10854,9 @@
       <c r="A33" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
       <c r="E33" s="47"/>
       <c r="F33" s="58" t="s">
         <v>70</v>
@@ -10893,7 +10893,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="49">
+      <c r="A35" s="51">
         <v>4</v>
       </c>
       <c r="B35" s="5">
@@ -18705,7 +18705,7 @@
   <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+      <selection activeCell="B136" sqref="B136:B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18725,9 +18725,9 @@
       <c r="A1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
@@ -18770,7 +18770,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="62">
+      <c r="A3" s="69">
         <v>22</v>
       </c>
       <c r="B3" s="31">
@@ -18800,7 +18800,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="31">
         <v>22.2</v>
       </c>
@@ -18822,7 +18822,7 @@
       <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="31">
         <v>22.3</v>
       </c>
@@ -18847,9 +18847,9 @@
       <c r="A7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="47"/>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -18886,7 +18886,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="62">
+      <c r="A9" s="69">
         <v>33</v>
       </c>
       <c r="B9" s="31">
@@ -18904,7 +18904,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="62"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="33">
         <v>33.200000000000003</v>
       </c>
@@ -18920,7 +18920,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="62"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="31">
         <v>33.299999999999997</v>
       </c>
@@ -18936,7 +18936,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="62"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="31">
         <v>33.4</v>
       </c>
@@ -18952,7 +18952,7 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="31">
         <v>33.5</v>
       </c>
@@ -18971,10 +18971,10 @@
       <c r="A15" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="64"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19164,7 +19164,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="67">
+      <c r="A27" s="62">
         <v>35</v>
       </c>
       <c r="B27" s="5">
@@ -19182,7 +19182,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="68"/>
+      <c r="A28" s="67"/>
       <c r="B28" s="31">
         <v>35.200000000000003</v>
       </c>
@@ -19198,7 +19198,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="68"/>
+      <c r="A29" s="67"/>
       <c r="B29" s="5">
         <v>35.299999999999997</v>
       </c>
@@ -19214,7 +19214,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="68"/>
+      <c r="A30" s="67"/>
       <c r="B30" s="31">
         <v>35.4</v>
       </c>
@@ -19230,7 +19230,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="68"/>
+      <c r="A31" s="67"/>
       <c r="B31" s="5">
         <v>35.5</v>
       </c>
@@ -19246,7 +19246,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="68"/>
+      <c r="A32" s="67"/>
       <c r="B32" s="31">
         <v>35.6</v>
       </c>
@@ -19262,7 +19262,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="68"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -19278,7 +19278,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="69"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="5">
         <v>35.799999999999997</v>
       </c>
@@ -19336,7 +19336,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="49">
+      <c r="A38" s="51">
         <v>40</v>
       </c>
       <c r="B38" s="5">
@@ -19508,7 +19508,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="49">
+      <c r="A49" s="51">
         <v>23</v>
       </c>
       <c r="B49" s="5">
@@ -19530,7 +19530,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="50"/>
+      <c r="A50" s="52"/>
       <c r="B50" s="5">
         <v>23.2</v>
       </c>
@@ -19550,7 +19550,7 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="50"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="5">
         <v>23.3</v>
       </c>
@@ -19570,7 +19570,7 @@
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="50"/>
+      <c r="A52" s="52"/>
       <c r="B52" s="5">
         <v>23.4</v>
       </c>
@@ -19590,7 +19590,7 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="50"/>
+      <c r="A53" s="52"/>
       <c r="B53" s="5">
         <v>23.5</v>
       </c>
@@ -19610,7 +19610,7 @@
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="50"/>
+      <c r="A54" s="52"/>
       <c r="B54" s="5">
         <v>23.6</v>
       </c>
@@ -19630,7 +19630,7 @@
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="50"/>
+      <c r="A55" s="52"/>
       <c r="B55" s="5">
         <v>23.7</v>
       </c>
@@ -19650,7 +19650,7 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="51"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="5">
         <v>23.8</v>
       </c>
@@ -19712,7 +19712,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="49">
+      <c r="A60" s="51">
         <v>3</v>
       </c>
       <c r="B60" s="5">
@@ -19730,7 +19730,7 @@
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="50"/>
+      <c r="A61" s="52"/>
       <c r="B61" s="5">
         <v>3.2</v>
       </c>
@@ -19746,7 +19746,7 @@
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="50"/>
+      <c r="A62" s="52"/>
       <c r="B62" s="5">
         <v>3.3</v>
       </c>
@@ -19762,7 +19762,7 @@
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="50"/>
+      <c r="A63" s="52"/>
       <c r="B63" s="5">
         <v>3.4</v>
       </c>
@@ -19778,7 +19778,7 @@
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="50"/>
+      <c r="A64" s="52"/>
       <c r="B64" s="5">
         <v>3.5</v>
       </c>
@@ -19794,7 +19794,7 @@
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="50"/>
+      <c r="A65" s="52"/>
       <c r="B65" s="5">
         <v>3.6</v>
       </c>
@@ -19810,7 +19810,7 @@
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="51"/>
+      <c r="A66" s="50"/>
       <c r="B66" s="5">
         <v>3.7</v>
       </c>
@@ -19868,7 +19868,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="49">
+      <c r="A70" s="51">
         <v>41</v>
       </c>
       <c r="B70" s="5">
@@ -19888,7 +19888,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="50"/>
+      <c r="A71" s="52"/>
       <c r="B71" s="5">
         <v>41.2</v>
       </c>
@@ -19906,7 +19906,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="50"/>
+      <c r="A72" s="52"/>
       <c r="B72" s="5">
         <v>41.3</v>
       </c>
@@ -19924,7 +19924,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="50"/>
+      <c r="A73" s="52"/>
       <c r="B73" s="5">
         <v>41.4</v>
       </c>
@@ -19942,7 +19942,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="50"/>
+      <c r="A74" s="52"/>
       <c r="B74" s="5">
         <v>41.5</v>
       </c>
@@ -19960,7 +19960,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="50"/>
+      <c r="A75" s="52"/>
       <c r="B75" s="5">
         <v>41.6</v>
       </c>
@@ -19978,7 +19978,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="51"/>
+      <c r="A76" s="50"/>
       <c r="B76" s="5">
         <v>41.7</v>
       </c>
@@ -20038,7 +20038,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="49">
+      <c r="A80" s="51">
         <v>25</v>
       </c>
       <c r="B80" s="5">
@@ -20060,7 +20060,7 @@
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="50"/>
+      <c r="A81" s="52"/>
       <c r="B81" s="5">
         <v>25.2</v>
       </c>
@@ -20080,7 +20080,7 @@
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="50"/>
+      <c r="A82" s="52"/>
       <c r="B82" s="5">
         <v>25.3</v>
       </c>
@@ -20100,7 +20100,7 @@
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="50"/>
+      <c r="A83" s="52"/>
       <c r="B83" s="5">
         <v>25.4</v>
       </c>
@@ -20120,7 +20120,7 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="50"/>
+      <c r="A84" s="52"/>
       <c r="B84" s="5">
         <v>25.5</v>
       </c>
@@ -20140,7 +20140,7 @@
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="50"/>
+      <c r="A85" s="52"/>
       <c r="B85" s="5">
         <v>25.6</v>
       </c>
@@ -20160,7 +20160,7 @@
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="50"/>
+      <c r="A86" s="52"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -20170,7 +20170,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="51"/>
+      <c r="A87" s="50"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -20222,7 +20222,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="49">
+      <c r="A91" s="51">
         <v>26</v>
       </c>
       <c r="B91" s="39">
@@ -20244,7 +20244,7 @@
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="50"/>
+      <c r="A92" s="52"/>
       <c r="B92" s="39">
         <v>26.2</v>
       </c>
@@ -20264,7 +20264,7 @@
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="50"/>
+      <c r="A93" s="52"/>
       <c r="B93" s="39">
         <v>26.3</v>
       </c>
@@ -20284,7 +20284,7 @@
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="50"/>
+      <c r="A94" s="52"/>
       <c r="B94" s="39">
         <v>26.4</v>
       </c>
@@ -20304,7 +20304,7 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="50"/>
+      <c r="A95" s="52"/>
       <c r="B95" s="39">
         <v>26.5</v>
       </c>
@@ -20324,7 +20324,7 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="50"/>
+      <c r="A96" s="52"/>
       <c r="B96" s="39">
         <v>26.6</v>
       </c>
@@ -20344,7 +20344,7 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="50"/>
+      <c r="A97" s="52"/>
       <c r="B97" s="39">
         <v>26.7</v>
       </c>
@@ -20364,7 +20364,7 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="50"/>
+      <c r="A98" s="52"/>
       <c r="B98" s="39">
         <v>26.8</v>
       </c>
@@ -20384,7 +20384,7 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="51"/>
+      <c r="A99" s="50"/>
       <c r="B99" s="39">
         <v>26.9</v>
       </c>
@@ -20446,7 +20446,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="49">
+      <c r="A103" s="51">
         <v>27</v>
       </c>
       <c r="B103" s="5">
@@ -20468,7 +20468,7 @@
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="50"/>
+      <c r="A104" s="52"/>
       <c r="B104" s="5">
         <v>27.2</v>
       </c>
@@ -20488,7 +20488,7 @@
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="50"/>
+      <c r="A105" s="52"/>
       <c r="B105" s="5">
         <v>27.3</v>
       </c>
@@ -20508,7 +20508,7 @@
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="50"/>
+      <c r="A106" s="52"/>
       <c r="B106" s="5">
         <v>27.4</v>
       </c>
@@ -20528,7 +20528,7 @@
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="50"/>
+      <c r="A107" s="52"/>
       <c r="B107" s="5">
         <v>27.5</v>
       </c>
@@ -20548,7 +20548,7 @@
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="50"/>
+      <c r="A108" s="52"/>
       <c r="B108" s="5">
         <v>27.6</v>
       </c>
@@ -20568,7 +20568,7 @@
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="51"/>
+      <c r="A109" s="50"/>
       <c r="B109" s="5">
         <v>27.7</v>
       </c>
@@ -20630,7 +20630,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="67">
+      <c r="A113" s="62">
         <v>4</v>
       </c>
       <c r="B113" s="31">
@@ -20650,7 +20650,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="70"/>
+      <c r="A114" s="63"/>
       <c r="B114" s="31">
         <v>4.2</v>
       </c>
@@ -20668,7 +20668,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="70"/>
+      <c r="A115" s="63"/>
       <c r="B115" s="31">
         <v>4.3</v>
       </c>
@@ -20686,7 +20686,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="70"/>
+      <c r="A116" s="63"/>
       <c r="B116" s="31">
         <v>4.4000000000000004</v>
       </c>
@@ -20704,7 +20704,7 @@
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="70"/>
+      <c r="A117" s="63"/>
       <c r="B117" s="31">
         <v>4.5</v>
       </c>
@@ -20722,7 +20722,7 @@
       <c r="H117" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="70"/>
+      <c r="A118" s="63"/>
       <c r="B118" s="31">
         <v>4.5999999999999996</v>
       </c>
@@ -20740,7 +20740,7 @@
       <c r="H118" s="3"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="70"/>
+      <c r="A119" s="63"/>
       <c r="B119" s="31">
         <v>4.7</v>
       </c>
@@ -20758,7 +20758,7 @@
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="70"/>
+      <c r="A120" s="63"/>
       <c r="B120" s="31">
         <v>4.8</v>
       </c>
@@ -20776,7 +20776,7 @@
       <c r="H120" s="3"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="70"/>
+      <c r="A121" s="63"/>
       <c r="B121" s="31">
         <v>4.9000000000000004</v>
       </c>
@@ -20794,7 +20794,7 @@
       <c r="H121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="71"/>
+      <c r="A122" s="64"/>
       <c r="B122" s="31">
         <v>5</v>
       </c>
@@ -20854,7 +20854,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="49">
+      <c r="A126" s="51">
         <v>30</v>
       </c>
       <c r="B126" s="5">
@@ -20874,7 +20874,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="50"/>
+      <c r="A127" s="52"/>
       <c r="B127" s="5">
         <v>27.2</v>
       </c>
@@ -20892,7 +20892,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="50"/>
+      <c r="A128" s="52"/>
       <c r="B128" s="5">
         <v>27.3</v>
       </c>
@@ -20910,7 +20910,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="50"/>
+      <c r="A129" s="52"/>
       <c r="B129" s="5">
         <v>27.4</v>
       </c>
@@ -20928,7 +20928,7 @@
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="50"/>
+      <c r="A130" s="52"/>
       <c r="B130" s="5">
         <v>27.5</v>
       </c>
@@ -20946,7 +20946,7 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="50"/>
+      <c r="A131" s="52"/>
       <c r="B131" s="5">
         <v>27.6</v>
       </c>
@@ -20964,7 +20964,7 @@
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="51"/>
+      <c r="A132" s="50"/>
       <c r="B132" s="5">
         <v>27.7</v>
       </c>
@@ -21024,7 +21024,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="49">
+      <c r="A136" s="51">
         <v>32</v>
       </c>
       <c r="B136" s="5">
@@ -21046,7 +21046,7 @@
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="50"/>
+      <c r="A137" s="52"/>
       <c r="B137" s="5">
         <v>32.200000000000003</v>
       </c>
@@ -21066,7 +21066,7 @@
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="50"/>
+      <c r="A138" s="52"/>
       <c r="B138" s="5">
         <v>32.299999999999997</v>
       </c>
@@ -21086,7 +21086,7 @@
       <c r="H138" s="3"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="50"/>
+      <c r="A139" s="52"/>
       <c r="B139" s="5">
         <v>32.4</v>
       </c>
@@ -21106,7 +21106,7 @@
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="50"/>
+      <c r="A140" s="52"/>
       <c r="B140" s="5">
         <v>32.5</v>
       </c>
@@ -21126,7 +21126,7 @@
       <c r="H140" s="3"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="50"/>
+      <c r="A141" s="52"/>
       <c r="B141" s="5">
         <v>32.6</v>
       </c>
@@ -21146,7 +21146,7 @@
       <c r="H141" s="3"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="51"/>
+      <c r="A142" s="50"/>
       <c r="B142" s="5">
         <v>32.700000000000003</v>
       </c>
@@ -21167,32 +21167,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:A122"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="A80:A87"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="G134:H134"/>
     <mergeCell ref="A136:A142"/>
@@ -21209,6 +21183,32 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="A80:A87"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:A122"/>
   </mergeCells>
   <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="27" priority="23">

</xml_diff>

<commit_message>
Revert "Revert "Moved events attending page""
This reverts commit 1b666387916a6799e8bde6542f4ac59905ffb53f.
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -788,18 +788,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -822,15 +822,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -839,11 +842,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1682,9 +1682,9 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>6.2</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>6.3</v>
       </c>
@@ -1815,7 +1815,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>6.4</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>6.5</v>
       </c>
@@ -1863,7 +1863,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="5">
         <v>6.6</v>
       </c>
@@ -1894,17 +1894,17 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="47"/>
       <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="52" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="47"/>
@@ -1938,7 +1938,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="51">
+      <c r="A12" s="49">
         <v>1</v>
       </c>
       <c r="B12" s="17">
@@ -1963,7 +1963,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="17">
         <v>1.2</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="17">
         <v>1.3</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="55">
         <v>1.4</v>
       </c>
@@ -2017,27 +2017,27 @@
       <c r="F15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="53">
         <v>42378</v>
       </c>
       <c r="H15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
       <c r="H16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="16">
         <v>1.5</v>
       </c>
@@ -2071,9 +2071,9 @@
       <c r="A19" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="47"/>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -2112,7 +2112,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51">
+      <c r="A21" s="49">
         <v>11</v>
       </c>
       <c r="B21" s="22">
@@ -2139,7 +2139,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="22">
         <v>11.2</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2186,9 +2186,9 @@
       <c r="A25" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="1" t="s">
         <v>42</v>
@@ -2227,7 +2227,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>12</v>
       </c>
       <c r="B27" s="22">
@@ -2254,7 +2254,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="22">
         <v>12.2</v>
       </c>
@@ -2277,7 +2277,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="22">
         <v>12.3</v>
       </c>
@@ -2320,9 +2320,9 @@
       <c r="A32" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="47"/>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -2361,7 +2361,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="51"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2372,7 +2372,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="52"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2383,7 +2383,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="52"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2394,7 +2394,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="52"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2405,7 +2405,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="52"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2416,7 +2416,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2427,7 +2427,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -10123,15 +10123,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G15:G16"/>
@@ -10143,6 +10134,15 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 A1 F10:G10 A10 F19:G19 A19 F25:G25 A25 F32:G32 A32">
     <cfRule type="notContainsBlanks" dxfId="37" priority="1">
@@ -10179,9 +10179,9 @@
       <c r="A1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="58" t="s">
         <v>1</v>
@@ -10227,7 +10227,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>21</v>
       </c>
       <c r="B3" s="5">
@@ -10260,7 +10260,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>21.2</v>
       </c>
@@ -10284,7 +10284,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>21.3</v>
       </c>
@@ -10308,7 +10308,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>21.4</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>21.5</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="5">
         <v>21.6</v>
       </c>
@@ -10376,7 +10376,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="5">
         <v>21.7</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="5">
         <v>21.8</v>
       </c>
@@ -10422,7 +10422,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="5">
         <v>21.9</v>
       </c>
@@ -10458,9 +10458,9 @@
       <c r="A13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="47"/>
       <c r="F13" s="58" t="s">
         <v>42</v>
@@ -10497,7 +10497,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="51">
+      <c r="A15" s="49">
         <v>20</v>
       </c>
       <c r="B15" s="5">
@@ -10521,7 +10521,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="5">
         <v>20.2</v>
       </c>
@@ -10543,7 +10543,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="5">
         <v>20.3</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -10600,9 +10600,9 @@
       <c r="A20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="47"/>
       <c r="F20" s="58" t="s">
         <v>49</v>
@@ -10639,7 +10639,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51">
+      <c r="A22" s="49">
         <v>5</v>
       </c>
       <c r="B22" s="5">
@@ -10661,7 +10661,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5">
         <v>5.2</v>
       </c>
@@ -10690,9 +10690,9 @@
       <c r="A25" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="58" t="s">
         <v>40</v>
@@ -10729,7 +10729,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>8</v>
       </c>
       <c r="B27" s="5">
@@ -10854,9 +10854,9 @@
       <c r="A33" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="47"/>
       <c r="F33" s="58" t="s">
         <v>70</v>
@@ -10893,7 +10893,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51">
+      <c r="A35" s="49">
         <v>4</v>
       </c>
       <c r="B35" s="5">
@@ -18705,7 +18705,7 @@
   <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136:B142"/>
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18725,9 +18725,9 @@
       <c r="A1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
@@ -18770,7 +18770,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="69">
+      <c r="A3" s="62">
         <v>22</v>
       </c>
       <c r="B3" s="31">
@@ -18800,7 +18800,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="69"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="31">
         <v>22.2</v>
       </c>
@@ -18822,7 +18822,7 @@
       <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="69"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="31">
         <v>22.3</v>
       </c>
@@ -18847,9 +18847,9 @@
       <c r="A7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="47"/>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -18886,7 +18886,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="69">
+      <c r="A9" s="62">
         <v>33</v>
       </c>
       <c r="B9" s="31">
@@ -18904,7 +18904,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="33">
         <v>33.200000000000003</v>
       </c>
@@ -18920,7 +18920,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="31">
         <v>33.299999999999997</v>
       </c>
@@ -18936,7 +18936,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="31">
         <v>33.4</v>
       </c>
@@ -18952,7 +18952,7 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="31">
         <v>33.5</v>
       </c>
@@ -18971,10 +18971,10 @@
       <c r="A15" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19164,7 +19164,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="62">
+      <c r="A27" s="67">
         <v>35</v>
       </c>
       <c r="B27" s="5">
@@ -19182,7 +19182,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="67"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="31">
         <v>35.200000000000003</v>
       </c>
@@ -19198,7 +19198,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="5">
         <v>35.299999999999997</v>
       </c>
@@ -19214,7 +19214,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="67"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="31">
         <v>35.4</v>
       </c>
@@ -19230,7 +19230,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="67"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="5">
         <v>35.5</v>
       </c>
@@ -19246,7 +19246,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="67"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="31">
         <v>35.6</v>
       </c>
@@ -19262,7 +19262,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="67"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -19278,7 +19278,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="68"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="5">
         <v>35.799999999999997</v>
       </c>
@@ -19336,7 +19336,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="51">
+      <c r="A38" s="49">
         <v>40</v>
       </c>
       <c r="B38" s="5">
@@ -19508,7 +19508,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="51">
+      <c r="A49" s="49">
         <v>23</v>
       </c>
       <c r="B49" s="5">
@@ -19530,7 +19530,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="52"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="5">
         <v>23.2</v>
       </c>
@@ -19550,7 +19550,7 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="52"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="5">
         <v>23.3</v>
       </c>
@@ -19570,7 +19570,7 @@
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="52"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="5">
         <v>23.4</v>
       </c>
@@ -19590,7 +19590,7 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="52"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="5">
         <v>23.5</v>
       </c>
@@ -19610,7 +19610,7 @@
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="52"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="5">
         <v>23.6</v>
       </c>
@@ -19630,7 +19630,7 @@
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="52"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="5">
         <v>23.7</v>
       </c>
@@ -19650,7 +19650,7 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="50"/>
+      <c r="A56" s="51"/>
       <c r="B56" s="5">
         <v>23.8</v>
       </c>
@@ -19712,7 +19712,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="51">
+      <c r="A60" s="49">
         <v>3</v>
       </c>
       <c r="B60" s="5">
@@ -19730,7 +19730,7 @@
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="5">
         <v>3.2</v>
       </c>
@@ -19746,7 +19746,7 @@
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="5">
         <v>3.3</v>
       </c>
@@ -19762,7 +19762,7 @@
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="5">
         <v>3.4</v>
       </c>
@@ -19778,7 +19778,7 @@
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
+      <c r="A64" s="50"/>
       <c r="B64" s="5">
         <v>3.5</v>
       </c>
@@ -19794,7 +19794,7 @@
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
+      <c r="A65" s="50"/>
       <c r="B65" s="5">
         <v>3.6</v>
       </c>
@@ -19810,7 +19810,7 @@
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="50"/>
+      <c r="A66" s="51"/>
       <c r="B66" s="5">
         <v>3.7</v>
       </c>
@@ -19868,7 +19868,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="51">
+      <c r="A70" s="49">
         <v>41</v>
       </c>
       <c r="B70" s="5">
@@ -19888,7 +19888,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="52"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="5">
         <v>41.2</v>
       </c>
@@ -19906,7 +19906,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="52"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="5">
         <v>41.3</v>
       </c>
@@ -19924,7 +19924,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="52"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="5">
         <v>41.4</v>
       </c>
@@ -19942,7 +19942,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="52"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="5">
         <v>41.5</v>
       </c>
@@ -19960,7 +19960,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
+      <c r="A75" s="50"/>
       <c r="B75" s="5">
         <v>41.6</v>
       </c>
@@ -19978,7 +19978,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="50"/>
+      <c r="A76" s="51"/>
       <c r="B76" s="5">
         <v>41.7</v>
       </c>
@@ -20038,7 +20038,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="51">
+      <c r="A80" s="49">
         <v>25</v>
       </c>
       <c r="B80" s="5">
@@ -20060,7 +20060,7 @@
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="52"/>
+      <c r="A81" s="50"/>
       <c r="B81" s="5">
         <v>25.2</v>
       </c>
@@ -20080,7 +20080,7 @@
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="52"/>
+      <c r="A82" s="50"/>
       <c r="B82" s="5">
         <v>25.3</v>
       </c>
@@ -20100,7 +20100,7 @@
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="52"/>
+      <c r="A83" s="50"/>
       <c r="B83" s="5">
         <v>25.4</v>
       </c>
@@ -20120,7 +20120,7 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="52"/>
+      <c r="A84" s="50"/>
       <c r="B84" s="5">
         <v>25.5</v>
       </c>
@@ -20140,7 +20140,7 @@
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="52"/>
+      <c r="A85" s="50"/>
       <c r="B85" s="5">
         <v>25.6</v>
       </c>
@@ -20160,7 +20160,7 @@
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="52"/>
+      <c r="A86" s="50"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -20170,7 +20170,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="50"/>
+      <c r="A87" s="51"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -20222,7 +20222,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="51">
+      <c r="A91" s="49">
         <v>26</v>
       </c>
       <c r="B91" s="39">
@@ -20244,7 +20244,7 @@
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="52"/>
+      <c r="A92" s="50"/>
       <c r="B92" s="39">
         <v>26.2</v>
       </c>
@@ -20264,7 +20264,7 @@
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="52"/>
+      <c r="A93" s="50"/>
       <c r="B93" s="39">
         <v>26.3</v>
       </c>
@@ -20284,7 +20284,7 @@
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="52"/>
+      <c r="A94" s="50"/>
       <c r="B94" s="39">
         <v>26.4</v>
       </c>
@@ -20304,7 +20304,7 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="52"/>
+      <c r="A95" s="50"/>
       <c r="B95" s="39">
         <v>26.5</v>
       </c>
@@ -20324,7 +20324,7 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="52"/>
+      <c r="A96" s="50"/>
       <c r="B96" s="39">
         <v>26.6</v>
       </c>
@@ -20344,7 +20344,7 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
+      <c r="A97" s="50"/>
       <c r="B97" s="39">
         <v>26.7</v>
       </c>
@@ -20364,7 +20364,7 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="52"/>
+      <c r="A98" s="50"/>
       <c r="B98" s="39">
         <v>26.8</v>
       </c>
@@ -20384,7 +20384,7 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="50"/>
+      <c r="A99" s="51"/>
       <c r="B99" s="39">
         <v>26.9</v>
       </c>
@@ -20446,7 +20446,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="51">
+      <c r="A103" s="49">
         <v>27</v>
       </c>
       <c r="B103" s="5">
@@ -20468,7 +20468,7 @@
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="52"/>
+      <c r="A104" s="50"/>
       <c r="B104" s="5">
         <v>27.2</v>
       </c>
@@ -20488,7 +20488,7 @@
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="52"/>
+      <c r="A105" s="50"/>
       <c r="B105" s="5">
         <v>27.3</v>
       </c>
@@ -20508,7 +20508,7 @@
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="52"/>
+      <c r="A106" s="50"/>
       <c r="B106" s="5">
         <v>27.4</v>
       </c>
@@ -20528,7 +20528,7 @@
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="52"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="5">
         <v>27.5</v>
       </c>
@@ -20548,7 +20548,7 @@
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="52"/>
+      <c r="A108" s="50"/>
       <c r="B108" s="5">
         <v>27.6</v>
       </c>
@@ -20568,7 +20568,7 @@
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="50"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="5">
         <v>27.7</v>
       </c>
@@ -20630,7 +20630,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="62">
+      <c r="A113" s="67">
         <v>4</v>
       </c>
       <c r="B113" s="31">
@@ -20650,7 +20650,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="63"/>
+      <c r="A114" s="70"/>
       <c r="B114" s="31">
         <v>4.2</v>
       </c>
@@ -20668,7 +20668,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="63"/>
+      <c r="A115" s="70"/>
       <c r="B115" s="31">
         <v>4.3</v>
       </c>
@@ -20686,7 +20686,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="63"/>
+      <c r="A116" s="70"/>
       <c r="B116" s="31">
         <v>4.4000000000000004</v>
       </c>
@@ -20704,7 +20704,7 @@
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="63"/>
+      <c r="A117" s="70"/>
       <c r="B117" s="31">
         <v>4.5</v>
       </c>
@@ -20722,7 +20722,7 @@
       <c r="H117" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="63"/>
+      <c r="A118" s="70"/>
       <c r="B118" s="31">
         <v>4.5999999999999996</v>
       </c>
@@ -20740,7 +20740,7 @@
       <c r="H118" s="3"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="63"/>
+      <c r="A119" s="70"/>
       <c r="B119" s="31">
         <v>4.7</v>
       </c>
@@ -20758,7 +20758,7 @@
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="63"/>
+      <c r="A120" s="70"/>
       <c r="B120" s="31">
         <v>4.8</v>
       </c>
@@ -20776,7 +20776,7 @@
       <c r="H120" s="3"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="63"/>
+      <c r="A121" s="70"/>
       <c r="B121" s="31">
         <v>4.9000000000000004</v>
       </c>
@@ -20794,7 +20794,7 @@
       <c r="H121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="64"/>
+      <c r="A122" s="71"/>
       <c r="B122" s="31">
         <v>5</v>
       </c>
@@ -20854,7 +20854,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="51">
+      <c r="A126" s="49">
         <v>30</v>
       </c>
       <c r="B126" s="5">
@@ -20874,7 +20874,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="52"/>
+      <c r="A127" s="50"/>
       <c r="B127" s="5">
         <v>27.2</v>
       </c>
@@ -20892,7 +20892,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="52"/>
+      <c r="A128" s="50"/>
       <c r="B128" s="5">
         <v>27.3</v>
       </c>
@@ -20910,7 +20910,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="52"/>
+      <c r="A129" s="50"/>
       <c r="B129" s="5">
         <v>27.4</v>
       </c>
@@ -20928,7 +20928,7 @@
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="52"/>
+      <c r="A130" s="50"/>
       <c r="B130" s="5">
         <v>27.5</v>
       </c>
@@ -20946,7 +20946,7 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="52"/>
+      <c r="A131" s="50"/>
       <c r="B131" s="5">
         <v>27.6</v>
       </c>
@@ -20964,7 +20964,7 @@
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="50"/>
+      <c r="A132" s="51"/>
       <c r="B132" s="5">
         <v>27.7</v>
       </c>
@@ -21024,7 +21024,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="51">
+      <c r="A136" s="49">
         <v>32</v>
       </c>
       <c r="B136" s="5">
@@ -21046,7 +21046,7 @@
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="52"/>
+      <c r="A137" s="50"/>
       <c r="B137" s="5">
         <v>32.200000000000003</v>
       </c>
@@ -21066,7 +21066,7 @@
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="52"/>
+      <c r="A138" s="50"/>
       <c r="B138" s="5">
         <v>32.299999999999997</v>
       </c>
@@ -21086,7 +21086,7 @@
       <c r="H138" s="3"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="52"/>
+      <c r="A139" s="50"/>
       <c r="B139" s="5">
         <v>32.4</v>
       </c>
@@ -21106,7 +21106,7 @@
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="52"/>
+      <c r="A140" s="50"/>
       <c r="B140" s="5">
         <v>32.5</v>
       </c>
@@ -21126,7 +21126,7 @@
       <c r="H140" s="3"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="52"/>
+      <c r="A141" s="50"/>
       <c r="B141" s="5">
         <v>32.6</v>
       </c>
@@ -21146,7 +21146,7 @@
       <c r="H141" s="3"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="50"/>
+      <c r="A142" s="51"/>
       <c r="B142" s="5">
         <v>32.700000000000003</v>
       </c>
@@ -21167,6 +21167,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="A80:A87"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="G134:H134"/>
     <mergeCell ref="A136:A142"/>
@@ -21183,32 +21209,6 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="G36:H36"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="A80:A87"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:A122"/>
   </mergeCells>
   <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="27" priority="23">

</xml_diff>

<commit_message>
Forgot to delete the taken time
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -788,18 +788,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -822,18 +822,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -842,8 +839,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1682,9 +1682,9 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49">
+      <c r="A3" s="51">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="50"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="5">
         <v>6.2</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="5">
         <v>6.3</v>
       </c>
@@ -1815,7 +1815,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="5">
         <v>6.4</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="5">
         <v>6.5</v>
       </c>
@@ -1863,7 +1863,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="5">
         <v>6.6</v>
       </c>
@@ -1894,17 +1894,17 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="47"/>
       <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="48" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="47"/>
@@ -1938,7 +1938,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49">
+      <c r="A12" s="51">
         <v>1</v>
       </c>
       <c r="B12" s="17">
@@ -1963,7 +1963,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="50"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="17">
         <v>1.2</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="50"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="17">
         <v>1.3</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="50"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="55">
         <v>1.4</v>
       </c>
@@ -2017,27 +2017,27 @@
       <c r="F15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="49">
         <v>42378</v>
       </c>
       <c r="H15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
       <c r="H16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="16">
         <v>1.5</v>
       </c>
@@ -2071,9 +2071,9 @@
       <c r="A19" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="47"/>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -2112,7 +2112,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49">
+      <c r="A21" s="51">
         <v>11</v>
       </c>
       <c r="B21" s="22">
@@ -2139,7 +2139,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="22">
         <v>11.2</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2186,9 +2186,9 @@
       <c r="A25" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="47"/>
       <c r="F25" s="1" t="s">
         <v>42</v>
@@ -2227,7 +2227,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49">
+      <c r="A27" s="51">
         <v>12</v>
       </c>
       <c r="B27" s="22">
@@ -2254,7 +2254,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="22">
         <v>12.2</v>
       </c>
@@ -2277,7 +2277,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="22">
         <v>12.3</v>
       </c>
@@ -2320,9 +2320,9 @@
       <c r="A32" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
       <c r="E32" s="47"/>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -2361,7 +2361,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="49"/>
+      <c r="A34" s="51"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2372,7 +2372,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="50"/>
+      <c r="A35" s="52"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2383,7 +2383,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="50"/>
+      <c r="A36" s="52"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2394,7 +2394,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="50"/>
+      <c r="A37" s="52"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2405,7 +2405,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="50"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2416,7 +2416,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="50"/>
+      <c r="A39" s="52"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2427,7 +2427,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="51"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -10123,6 +10123,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G15:G16"/>
@@ -10134,15 +10143,6 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 A1 F10:G10 A10 F19:G19 A19 F25:G25 A25 F32:G32 A32">
     <cfRule type="notContainsBlanks" dxfId="37" priority="1">
@@ -10179,9 +10179,9 @@
       <c r="A1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="47"/>
       <c r="F1" s="58" t="s">
         <v>1</v>
@@ -10227,7 +10227,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49">
+      <c r="A3" s="51">
         <v>21</v>
       </c>
       <c r="B3" s="5">
@@ -10260,7 +10260,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="50"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="5">
         <v>21.2</v>
       </c>
@@ -10284,7 +10284,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="5">
         <v>21.3</v>
       </c>
@@ -10308,7 +10308,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="5">
         <v>21.4</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="5">
         <v>21.5</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="5">
         <v>21.6</v>
       </c>
@@ -10376,7 +10376,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="50"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="5">
         <v>21.7</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="50"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="5">
         <v>21.8</v>
       </c>
@@ -10422,7 +10422,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="5">
         <v>21.9</v>
       </c>
@@ -10458,9 +10458,9 @@
       <c r="A13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="47"/>
       <c r="F13" s="58" t="s">
         <v>42</v>
@@ -10497,7 +10497,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49">
+      <c r="A15" s="51">
         <v>20</v>
       </c>
       <c r="B15" s="5">
@@ -10521,7 +10521,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="50"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="5">
         <v>20.2</v>
       </c>
@@ -10543,7 +10543,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="5">
         <v>20.3</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="51"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -10600,9 +10600,9 @@
       <c r="A20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="47"/>
       <c r="F20" s="58" t="s">
         <v>49</v>
@@ -10639,7 +10639,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49">
+      <c r="A22" s="51">
         <v>5</v>
       </c>
       <c r="B22" s="5">
@@ -10661,7 +10661,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="5">
         <v>5.2</v>
       </c>
@@ -10690,9 +10690,9 @@
       <c r="A25" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="47"/>
       <c r="F25" s="58" t="s">
         <v>40</v>
@@ -10729,7 +10729,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49">
+      <c r="A27" s="51">
         <v>8</v>
       </c>
       <c r="B27" s="5">
@@ -10854,9 +10854,9 @@
       <c r="A33" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
       <c r="E33" s="47"/>
       <c r="F33" s="58" t="s">
         <v>70</v>
@@ -10893,7 +10893,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="49">
+      <c r="A35" s="51">
         <v>4</v>
       </c>
       <c r="B35" s="5">
@@ -18705,7 +18705,7 @@
   <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+      <selection activeCell="E136" sqref="E136:E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18725,9 +18725,9 @@
       <c r="A1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
@@ -18770,7 +18770,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="62">
+      <c r="A3" s="69">
         <v>22</v>
       </c>
       <c r="B3" s="31">
@@ -18800,7 +18800,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="31">
         <v>22.2</v>
       </c>
@@ -18822,7 +18822,7 @@
       <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="31">
         <v>22.3</v>
       </c>
@@ -18847,9 +18847,9 @@
       <c r="A7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="47"/>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -18886,7 +18886,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="62">
+      <c r="A9" s="69">
         <v>33</v>
       </c>
       <c r="B9" s="31">
@@ -18904,7 +18904,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="62"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="33">
         <v>33.200000000000003</v>
       </c>
@@ -18920,7 +18920,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="62"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="31">
         <v>33.299999999999997</v>
       </c>
@@ -18936,7 +18936,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="62"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="31">
         <v>33.4</v>
       </c>
@@ -18952,7 +18952,7 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="31">
         <v>33.5</v>
       </c>
@@ -18971,10 +18971,10 @@
       <c r="A15" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="64"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19164,7 +19164,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="67">
+      <c r="A27" s="62">
         <v>35</v>
       </c>
       <c r="B27" s="5">
@@ -19182,7 +19182,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="68"/>
+      <c r="A28" s="67"/>
       <c r="B28" s="31">
         <v>35.200000000000003</v>
       </c>
@@ -19198,7 +19198,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="68"/>
+      <c r="A29" s="67"/>
       <c r="B29" s="5">
         <v>35.299999999999997</v>
       </c>
@@ -19214,7 +19214,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="68"/>
+      <c r="A30" s="67"/>
       <c r="B30" s="31">
         <v>35.4</v>
       </c>
@@ -19230,7 +19230,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="68"/>
+      <c r="A31" s="67"/>
       <c r="B31" s="5">
         <v>35.5</v>
       </c>
@@ -19246,7 +19246,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="68"/>
+      <c r="A32" s="67"/>
       <c r="B32" s="31">
         <v>35.6</v>
       </c>
@@ -19262,7 +19262,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="68"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -19278,7 +19278,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="69"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="5">
         <v>35.799999999999997</v>
       </c>
@@ -19336,7 +19336,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="49">
+      <c r="A38" s="51">
         <v>40</v>
       </c>
       <c r="B38" s="5">
@@ -19508,7 +19508,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="49">
+      <c r="A49" s="51">
         <v>23</v>
       </c>
       <c r="B49" s="5">
@@ -19530,7 +19530,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="50"/>
+      <c r="A50" s="52"/>
       <c r="B50" s="5">
         <v>23.2</v>
       </c>
@@ -19550,7 +19550,7 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="50"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="5">
         <v>23.3</v>
       </c>
@@ -19570,7 +19570,7 @@
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="50"/>
+      <c r="A52" s="52"/>
       <c r="B52" s="5">
         <v>23.4</v>
       </c>
@@ -19590,7 +19590,7 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="50"/>
+      <c r="A53" s="52"/>
       <c r="B53" s="5">
         <v>23.5</v>
       </c>
@@ -19610,7 +19610,7 @@
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="50"/>
+      <c r="A54" s="52"/>
       <c r="B54" s="5">
         <v>23.6</v>
       </c>
@@ -19630,7 +19630,7 @@
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="50"/>
+      <c r="A55" s="52"/>
       <c r="B55" s="5">
         <v>23.7</v>
       </c>
@@ -19650,7 +19650,7 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="51"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="5">
         <v>23.8</v>
       </c>
@@ -19712,7 +19712,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="49">
+      <c r="A60" s="51">
         <v>3</v>
       </c>
       <c r="B60" s="5">
@@ -19730,7 +19730,7 @@
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="50"/>
+      <c r="A61" s="52"/>
       <c r="B61" s="5">
         <v>3.2</v>
       </c>
@@ -19746,7 +19746,7 @@
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="50"/>
+      <c r="A62" s="52"/>
       <c r="B62" s="5">
         <v>3.3</v>
       </c>
@@ -19762,7 +19762,7 @@
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="50"/>
+      <c r="A63" s="52"/>
       <c r="B63" s="5">
         <v>3.4</v>
       </c>
@@ -19778,7 +19778,7 @@
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="50"/>
+      <c r="A64" s="52"/>
       <c r="B64" s="5">
         <v>3.5</v>
       </c>
@@ -19794,7 +19794,7 @@
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="50"/>
+      <c r="A65" s="52"/>
       <c r="B65" s="5">
         <v>3.6</v>
       </c>
@@ -19810,7 +19810,7 @@
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="51"/>
+      <c r="A66" s="50"/>
       <c r="B66" s="5">
         <v>3.7</v>
       </c>
@@ -19868,7 +19868,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="49">
+      <c r="A70" s="51">
         <v>41</v>
       </c>
       <c r="B70" s="5">
@@ -19888,7 +19888,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="50"/>
+      <c r="A71" s="52"/>
       <c r="B71" s="5">
         <v>41.2</v>
       </c>
@@ -19906,7 +19906,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="50"/>
+      <c r="A72" s="52"/>
       <c r="B72" s="5">
         <v>41.3</v>
       </c>
@@ -19924,7 +19924,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="50"/>
+      <c r="A73" s="52"/>
       <c r="B73" s="5">
         <v>41.4</v>
       </c>
@@ -19942,7 +19942,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="50"/>
+      <c r="A74" s="52"/>
       <c r="B74" s="5">
         <v>41.5</v>
       </c>
@@ -19960,7 +19960,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="50"/>
+      <c r="A75" s="52"/>
       <c r="B75" s="5">
         <v>41.6</v>
       </c>
@@ -19978,7 +19978,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="51"/>
+      <c r="A76" s="50"/>
       <c r="B76" s="5">
         <v>41.7</v>
       </c>
@@ -20038,7 +20038,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="49">
+      <c r="A80" s="51">
         <v>25</v>
       </c>
       <c r="B80" s="5">
@@ -20060,7 +20060,7 @@
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="50"/>
+      <c r="A81" s="52"/>
       <c r="B81" s="5">
         <v>25.2</v>
       </c>
@@ -20080,7 +20080,7 @@
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="50"/>
+      <c r="A82" s="52"/>
       <c r="B82" s="5">
         <v>25.3</v>
       </c>
@@ -20100,7 +20100,7 @@
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="50"/>
+      <c r="A83" s="52"/>
       <c r="B83" s="5">
         <v>25.4</v>
       </c>
@@ -20120,7 +20120,7 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="50"/>
+      <c r="A84" s="52"/>
       <c r="B84" s="5">
         <v>25.5</v>
       </c>
@@ -20140,7 +20140,7 @@
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="50"/>
+      <c r="A85" s="52"/>
       <c r="B85" s="5">
         <v>25.6</v>
       </c>
@@ -20160,7 +20160,7 @@
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="50"/>
+      <c r="A86" s="52"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -20170,7 +20170,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="51"/>
+      <c r="A87" s="50"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -20222,7 +20222,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="49">
+      <c r="A91" s="51">
         <v>26</v>
       </c>
       <c r="B91" s="39">
@@ -20244,7 +20244,7 @@
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="50"/>
+      <c r="A92" s="52"/>
       <c r="B92" s="39">
         <v>26.2</v>
       </c>
@@ -20264,7 +20264,7 @@
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="50"/>
+      <c r="A93" s="52"/>
       <c r="B93" s="39">
         <v>26.3</v>
       </c>
@@ -20284,7 +20284,7 @@
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="50"/>
+      <c r="A94" s="52"/>
       <c r="B94" s="39">
         <v>26.4</v>
       </c>
@@ -20304,7 +20304,7 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="50"/>
+      <c r="A95" s="52"/>
       <c r="B95" s="39">
         <v>26.5</v>
       </c>
@@ -20324,7 +20324,7 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="50"/>
+      <c r="A96" s="52"/>
       <c r="B96" s="39">
         <v>26.6</v>
       </c>
@@ -20344,7 +20344,7 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="50"/>
+      <c r="A97" s="52"/>
       <c r="B97" s="39">
         <v>26.7</v>
       </c>
@@ -20364,7 +20364,7 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="50"/>
+      <c r="A98" s="52"/>
       <c r="B98" s="39">
         <v>26.8</v>
       </c>
@@ -20384,7 +20384,7 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="51"/>
+      <c r="A99" s="50"/>
       <c r="B99" s="39">
         <v>26.9</v>
       </c>
@@ -20446,7 +20446,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="49">
+      <c r="A103" s="51">
         <v>27</v>
       </c>
       <c r="B103" s="5">
@@ -20468,7 +20468,7 @@
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="50"/>
+      <c r="A104" s="52"/>
       <c r="B104" s="5">
         <v>27.2</v>
       </c>
@@ -20488,7 +20488,7 @@
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="50"/>
+      <c r="A105" s="52"/>
       <c r="B105" s="5">
         <v>27.3</v>
       </c>
@@ -20508,7 +20508,7 @@
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="50"/>
+      <c r="A106" s="52"/>
       <c r="B106" s="5">
         <v>27.4</v>
       </c>
@@ -20528,7 +20528,7 @@
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="50"/>
+      <c r="A107" s="52"/>
       <c r="B107" s="5">
         <v>27.5</v>
       </c>
@@ -20548,7 +20548,7 @@
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="50"/>
+      <c r="A108" s="52"/>
       <c r="B108" s="5">
         <v>27.6</v>
       </c>
@@ -20568,7 +20568,7 @@
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="51"/>
+      <c r="A109" s="50"/>
       <c r="B109" s="5">
         <v>27.7</v>
       </c>
@@ -20630,7 +20630,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="67">
+      <c r="A113" s="62">
         <v>4</v>
       </c>
       <c r="B113" s="31">
@@ -20650,7 +20650,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="70"/>
+      <c r="A114" s="63"/>
       <c r="B114" s="31">
         <v>4.2</v>
       </c>
@@ -20668,7 +20668,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="70"/>
+      <c r="A115" s="63"/>
       <c r="B115" s="31">
         <v>4.3</v>
       </c>
@@ -20686,7 +20686,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="70"/>
+      <c r="A116" s="63"/>
       <c r="B116" s="31">
         <v>4.4000000000000004</v>
       </c>
@@ -20704,7 +20704,7 @@
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="70"/>
+      <c r="A117" s="63"/>
       <c r="B117" s="31">
         <v>4.5</v>
       </c>
@@ -20722,7 +20722,7 @@
       <c r="H117" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="70"/>
+      <c r="A118" s="63"/>
       <c r="B118" s="31">
         <v>4.5999999999999996</v>
       </c>
@@ -20740,7 +20740,7 @@
       <c r="H118" s="3"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="70"/>
+      <c r="A119" s="63"/>
       <c r="B119" s="31">
         <v>4.7</v>
       </c>
@@ -20758,7 +20758,7 @@
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="70"/>
+      <c r="A120" s="63"/>
       <c r="B120" s="31">
         <v>4.8</v>
       </c>
@@ -20776,7 +20776,7 @@
       <c r="H120" s="3"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="70"/>
+      <c r="A121" s="63"/>
       <c r="B121" s="31">
         <v>4.9000000000000004</v>
       </c>
@@ -20794,7 +20794,7 @@
       <c r="H121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="71"/>
+      <c r="A122" s="64"/>
       <c r="B122" s="31">
         <v>5</v>
       </c>
@@ -20854,7 +20854,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="49">
+      <c r="A126" s="51">
         <v>30</v>
       </c>
       <c r="B126" s="5">
@@ -20874,7 +20874,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="50"/>
+      <c r="A127" s="52"/>
       <c r="B127" s="5">
         <v>27.2</v>
       </c>
@@ -20892,7 +20892,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="50"/>
+      <c r="A128" s="52"/>
       <c r="B128" s="5">
         <v>27.3</v>
       </c>
@@ -20910,7 +20910,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="50"/>
+      <c r="A129" s="52"/>
       <c r="B129" s="5">
         <v>27.4</v>
       </c>
@@ -20928,7 +20928,7 @@
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="50"/>
+      <c r="A130" s="52"/>
       <c r="B130" s="5">
         <v>27.5</v>
       </c>
@@ -20946,7 +20946,7 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="50"/>
+      <c r="A131" s="52"/>
       <c r="B131" s="5">
         <v>27.6</v>
       </c>
@@ -20964,7 +20964,7 @@
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="51"/>
+      <c r="A132" s="50"/>
       <c r="B132" s="5">
         <v>27.7</v>
       </c>
@@ -21024,7 +21024,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="49">
+      <c r="A136" s="51">
         <v>32</v>
       </c>
       <c r="B136" s="5">
@@ -21036,9 +21036,7 @@
       <c r="D136" s="5">
         <v>1</v>
       </c>
-      <c r="E136" s="5">
-        <v>2</v>
-      </c>
+      <c r="E136" s="5"/>
       <c r="F136" s="27" t="s">
         <v>17</v>
       </c>
@@ -21046,7 +21044,7 @@
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="50"/>
+      <c r="A137" s="52"/>
       <c r="B137" s="5">
         <v>32.200000000000003</v>
       </c>
@@ -21056,9 +21054,7 @@
       <c r="D137" s="5">
         <v>0.5</v>
       </c>
-      <c r="E137" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="E137" s="5"/>
       <c r="F137" s="27" t="s">
         <v>17</v>
       </c>
@@ -21066,7 +21062,7 @@
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="50"/>
+      <c r="A138" s="52"/>
       <c r="B138" s="5">
         <v>32.299999999999997</v>
       </c>
@@ -21076,9 +21072,7 @@
       <c r="D138" s="5">
         <v>2</v>
       </c>
-      <c r="E138" s="5">
-        <v>1</v>
-      </c>
+      <c r="E138" s="5"/>
       <c r="F138" s="27" t="s">
         <v>17</v>
       </c>
@@ -21086,7 +21080,7 @@
       <c r="H138" s="3"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="50"/>
+      <c r="A139" s="52"/>
       <c r="B139" s="5">
         <v>32.4</v>
       </c>
@@ -21096,9 +21090,7 @@
       <c r="D139" s="5">
         <v>0.5</v>
       </c>
-      <c r="E139" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="E139" s="5"/>
       <c r="F139" s="27" t="s">
         <v>17</v>
       </c>
@@ -21106,7 +21098,7 @@
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="50"/>
+      <c r="A140" s="52"/>
       <c r="B140" s="5">
         <v>32.5</v>
       </c>
@@ -21116,9 +21108,7 @@
       <c r="D140" s="5">
         <v>3</v>
       </c>
-      <c r="E140" s="5">
-        <v>2</v>
-      </c>
+      <c r="E140" s="5"/>
       <c r="F140" s="27" t="s">
         <v>17</v>
       </c>
@@ -21126,7 +21116,7 @@
       <c r="H140" s="3"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="50"/>
+      <c r="A141" s="52"/>
       <c r="B141" s="5">
         <v>32.6</v>
       </c>
@@ -21136,9 +21126,7 @@
       <c r="D141" s="5">
         <v>1</v>
       </c>
-      <c r="E141" s="5">
-        <v>1</v>
-      </c>
+      <c r="E141" s="5"/>
       <c r="F141" s="27" t="s">
         <v>17</v>
       </c>
@@ -21146,7 +21134,7 @@
       <c r="H141" s="3"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="51"/>
+      <c r="A142" s="50"/>
       <c r="B142" s="5">
         <v>32.700000000000003</v>
       </c>
@@ -21156,9 +21144,7 @@
       <c r="D142" s="3">
         <v>0.5</v>
       </c>
-      <c r="E142" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="E142" s="3"/>
       <c r="F142" s="27" t="s">
         <v>17</v>
       </c>
@@ -21167,32 +21153,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:A122"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="A80:A87"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="G134:H134"/>
     <mergeCell ref="A136:A142"/>
@@ -21209,6 +21169,32 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="A80:A87"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:A122"/>
   </mergeCells>
   <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="27" priority="23">

</xml_diff>

<commit_message>
Forgot to add date completed
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -788,18 +788,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -822,15 +822,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -839,11 +842,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1682,9 +1682,9 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>6.2</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>6.3</v>
       </c>
@@ -1815,7 +1815,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>6.4</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>6.5</v>
       </c>
@@ -1863,7 +1863,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="5">
         <v>6.6</v>
       </c>
@@ -1894,17 +1894,17 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="47"/>
       <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="52" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="47"/>
@@ -1938,7 +1938,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="51">
+      <c r="A12" s="49">
         <v>1</v>
       </c>
       <c r="B12" s="17">
@@ -1963,7 +1963,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="17">
         <v>1.2</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="17">
         <v>1.3</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="55">
         <v>1.4</v>
       </c>
@@ -2017,27 +2017,27 @@
       <c r="F15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="53">
         <v>42378</v>
       </c>
       <c r="H15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
       <c r="H16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="16">
         <v>1.5</v>
       </c>
@@ -2071,9 +2071,9 @@
       <c r="A19" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="47"/>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -2112,7 +2112,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51">
+      <c r="A21" s="49">
         <v>11</v>
       </c>
       <c r="B21" s="22">
@@ -2139,7 +2139,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="22">
         <v>11.2</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2186,9 +2186,9 @@
       <c r="A25" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="1" t="s">
         <v>42</v>
@@ -2227,7 +2227,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>12</v>
       </c>
       <c r="B27" s="22">
@@ -2254,7 +2254,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="22">
         <v>12.2</v>
       </c>
@@ -2277,7 +2277,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="22">
         <v>12.3</v>
       </c>
@@ -2320,9 +2320,9 @@
       <c r="A32" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="47"/>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -2361,7 +2361,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="51"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2372,7 +2372,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="52"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2383,7 +2383,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="52"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2394,7 +2394,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="52"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2405,7 +2405,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="52"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2416,7 +2416,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2427,7 +2427,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -10123,15 +10123,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G15:G16"/>
@@ -10143,6 +10134,15 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 A1 F10:G10 A10 F19:G19 A19 F25:G25 A25 F32:G32 A32">
     <cfRule type="notContainsBlanks" dxfId="37" priority="1">
@@ -10179,9 +10179,9 @@
       <c r="A1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="58" t="s">
         <v>1</v>
@@ -10227,7 +10227,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>21</v>
       </c>
       <c r="B3" s="5">
@@ -10260,7 +10260,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>21.2</v>
       </c>
@@ -10284,7 +10284,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>21.3</v>
       </c>
@@ -10308,7 +10308,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>21.4</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>21.5</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="5">
         <v>21.6</v>
       </c>
@@ -10376,7 +10376,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="5">
         <v>21.7</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="5">
         <v>21.8</v>
       </c>
@@ -10422,7 +10422,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="5">
         <v>21.9</v>
       </c>
@@ -10458,9 +10458,9 @@
       <c r="A13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="47"/>
       <c r="F13" s="58" t="s">
         <v>42</v>
@@ -10497,7 +10497,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="51">
+      <c r="A15" s="49">
         <v>20</v>
       </c>
       <c r="B15" s="5">
@@ -10521,7 +10521,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="5">
         <v>20.2</v>
       </c>
@@ -10543,7 +10543,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="5">
         <v>20.3</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -10600,9 +10600,9 @@
       <c r="A20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="47"/>
       <c r="F20" s="58" t="s">
         <v>49</v>
@@ -10639,7 +10639,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51">
+      <c r="A22" s="49">
         <v>5</v>
       </c>
       <c r="B22" s="5">
@@ -10661,7 +10661,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5">
         <v>5.2</v>
       </c>
@@ -10690,9 +10690,9 @@
       <c r="A25" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="58" t="s">
         <v>40</v>
@@ -10729,7 +10729,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>8</v>
       </c>
       <c r="B27" s="5">
@@ -10854,9 +10854,9 @@
       <c r="A33" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="47"/>
       <c r="F33" s="58" t="s">
         <v>70</v>
@@ -10893,7 +10893,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51">
+      <c r="A35" s="49">
         <v>4</v>
       </c>
       <c r="B35" s="5">
@@ -18704,8 +18704,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136:E142"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103:G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18725,9 +18725,9 @@
       <c r="A1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
@@ -18770,7 +18770,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="69">
+      <c r="A3" s="62">
         <v>22</v>
       </c>
       <c r="B3" s="31">
@@ -18800,7 +18800,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="69"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="31">
         <v>22.2</v>
       </c>
@@ -18822,7 +18822,7 @@
       <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="69"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="31">
         <v>22.3</v>
       </c>
@@ -18847,9 +18847,9 @@
       <c r="A7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="47"/>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -18886,7 +18886,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="69">
+      <c r="A9" s="62">
         <v>33</v>
       </c>
       <c r="B9" s="31">
@@ -18904,7 +18904,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="33">
         <v>33.200000000000003</v>
       </c>
@@ -18920,7 +18920,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="31">
         <v>33.299999999999997</v>
       </c>
@@ -18936,7 +18936,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="31">
         <v>33.4</v>
       </c>
@@ -18952,7 +18952,7 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="31">
         <v>33.5</v>
       </c>
@@ -18971,10 +18971,10 @@
       <c r="A15" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19164,7 +19164,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="62">
+      <c r="A27" s="67">
         <v>35</v>
       </c>
       <c r="B27" s="5">
@@ -19182,7 +19182,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="67"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="31">
         <v>35.200000000000003</v>
       </c>
@@ -19198,7 +19198,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="5">
         <v>35.299999999999997</v>
       </c>
@@ -19214,7 +19214,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="67"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="31">
         <v>35.4</v>
       </c>
@@ -19230,7 +19230,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="67"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="5">
         <v>35.5</v>
       </c>
@@ -19246,7 +19246,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="67"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="31">
         <v>35.6</v>
       </c>
@@ -19262,7 +19262,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="67"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -19278,7 +19278,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="68"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="5">
         <v>35.799999999999997</v>
       </c>
@@ -19336,7 +19336,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="51">
+      <c r="A38" s="49">
         <v>40</v>
       </c>
       <c r="B38" s="5">
@@ -19508,7 +19508,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="51">
+      <c r="A49" s="49">
         <v>23</v>
       </c>
       <c r="B49" s="5">
@@ -19526,11 +19526,13 @@
       <c r="F49" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G49" s="5"/>
+      <c r="G49" s="10">
+        <v>42637</v>
+      </c>
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="52"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="5">
         <v>23.2</v>
       </c>
@@ -19546,11 +19548,13 @@
       <c r="F50" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="5"/>
+      <c r="G50" s="10">
+        <v>42637</v>
+      </c>
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="52"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="5">
         <v>23.3</v>
       </c>
@@ -19566,11 +19570,13 @@
       <c r="F51" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G51" s="5"/>
+      <c r="G51" s="10">
+        <v>42637</v>
+      </c>
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="52"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="5">
         <v>23.4</v>
       </c>
@@ -19586,11 +19592,13 @@
       <c r="F52" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G52" s="5"/>
+      <c r="G52" s="10">
+        <v>42637</v>
+      </c>
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="52"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="5">
         <v>23.5</v>
       </c>
@@ -19606,11 +19614,13 @@
       <c r="F53" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G53" s="5"/>
+      <c r="G53" s="10">
+        <v>42637</v>
+      </c>
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="52"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="5">
         <v>23.6</v>
       </c>
@@ -19626,11 +19636,13 @@
       <c r="F54" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G54" s="5"/>
+      <c r="G54" s="10">
+        <v>42637</v>
+      </c>
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="52"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="5">
         <v>23.7</v>
       </c>
@@ -19646,11 +19658,13 @@
       <c r="F55" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G55" s="5"/>
+      <c r="G55" s="10">
+        <v>42637</v>
+      </c>
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="50"/>
+      <c r="A56" s="51"/>
       <c r="B56" s="5">
         <v>23.8</v>
       </c>
@@ -19666,7 +19680,9 @@
       <c r="F56" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G56" s="3"/>
+      <c r="G56" s="10">
+        <v>42637</v>
+      </c>
       <c r="H56" s="3"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -19712,7 +19728,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="51">
+      <c r="A60" s="49">
         <v>3</v>
       </c>
       <c r="B60" s="5">
@@ -19730,7 +19746,7 @@
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="5">
         <v>3.2</v>
       </c>
@@ -19746,7 +19762,7 @@
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="5">
         <v>3.3</v>
       </c>
@@ -19762,7 +19778,7 @@
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="5">
         <v>3.4</v>
       </c>
@@ -19778,7 +19794,7 @@
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
+      <c r="A64" s="50"/>
       <c r="B64" s="5">
         <v>3.5</v>
       </c>
@@ -19794,7 +19810,7 @@
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
+      <c r="A65" s="50"/>
       <c r="B65" s="5">
         <v>3.6</v>
       </c>
@@ -19810,7 +19826,7 @@
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="50"/>
+      <c r="A66" s="51"/>
       <c r="B66" s="5">
         <v>3.7</v>
       </c>
@@ -19868,7 +19884,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="51">
+      <c r="A70" s="49">
         <v>41</v>
       </c>
       <c r="B70" s="5">
@@ -19888,7 +19904,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="52"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="5">
         <v>41.2</v>
       </c>
@@ -19906,7 +19922,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="52"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="5">
         <v>41.3</v>
       </c>
@@ -19924,7 +19940,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="52"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="5">
         <v>41.4</v>
       </c>
@@ -19942,7 +19958,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="52"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="5">
         <v>41.5</v>
       </c>
@@ -19960,7 +19976,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
+      <c r="A75" s="50"/>
       <c r="B75" s="5">
         <v>41.6</v>
       </c>
@@ -19978,7 +19994,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="50"/>
+      <c r="A76" s="51"/>
       <c r="B76" s="5">
         <v>41.7</v>
       </c>
@@ -20038,7 +20054,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="51">
+      <c r="A80" s="49">
         <v>25</v>
       </c>
       <c r="B80" s="5">
@@ -20056,11 +20072,13 @@
       <c r="F80" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G80" s="5"/>
+      <c r="G80" s="10">
+        <v>42636</v>
+      </c>
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="52"/>
+      <c r="A81" s="50"/>
       <c r="B81" s="5">
         <v>25.2</v>
       </c>
@@ -20076,11 +20094,13 @@
       <c r="F81" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G81" s="5"/>
+      <c r="G81" s="10">
+        <v>42636</v>
+      </c>
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="52"/>
+      <c r="A82" s="50"/>
       <c r="B82" s="5">
         <v>25.3</v>
       </c>
@@ -20096,11 +20116,13 @@
       <c r="F82" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G82" s="5"/>
+      <c r="G82" s="10">
+        <v>42636</v>
+      </c>
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="52"/>
+      <c r="A83" s="50"/>
       <c r="B83" s="5">
         <v>25.4</v>
       </c>
@@ -20116,11 +20138,13 @@
       <c r="F83" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G83" s="5"/>
+      <c r="G83" s="10">
+        <v>42636</v>
+      </c>
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="52"/>
+      <c r="A84" s="50"/>
       <c r="B84" s="5">
         <v>25.5</v>
       </c>
@@ -20136,11 +20160,13 @@
       <c r="F84" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G84" s="5"/>
+      <c r="G84" s="10">
+        <v>42636</v>
+      </c>
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="52"/>
+      <c r="A85" s="50"/>
       <c r="B85" s="5">
         <v>25.6</v>
       </c>
@@ -20156,11 +20182,13 @@
       <c r="F85" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G85" s="5"/>
+      <c r="G85" s="10">
+        <v>42636</v>
+      </c>
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="52"/>
+      <c r="A86" s="50"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -20170,7 +20198,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="50"/>
+      <c r="A87" s="51"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -20222,7 +20250,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="51">
+      <c r="A91" s="49">
         <v>26</v>
       </c>
       <c r="B91" s="39">
@@ -20240,11 +20268,13 @@
       <c r="F91" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G91" s="5"/>
+      <c r="G91" s="10">
+        <v>42636</v>
+      </c>
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="52"/>
+      <c r="A92" s="50"/>
       <c r="B92" s="39">
         <v>26.2</v>
       </c>
@@ -20260,11 +20290,13 @@
       <c r="F92" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G92" s="5"/>
+      <c r="G92" s="10">
+        <v>42636</v>
+      </c>
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="52"/>
+      <c r="A93" s="50"/>
       <c r="B93" s="39">
         <v>26.3</v>
       </c>
@@ -20280,11 +20312,13 @@
       <c r="F93" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G93" s="5"/>
+      <c r="G93" s="10">
+        <v>42636</v>
+      </c>
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="52"/>
+      <c r="A94" s="50"/>
       <c r="B94" s="39">
         <v>26.4</v>
       </c>
@@ -20300,11 +20334,13 @@
       <c r="F94" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G94" s="5"/>
+      <c r="G94" s="10">
+        <v>42636</v>
+      </c>
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="52"/>
+      <c r="A95" s="50"/>
       <c r="B95" s="39">
         <v>26.5</v>
       </c>
@@ -20320,11 +20356,13 @@
       <c r="F95" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G95" s="5"/>
+      <c r="G95" s="10">
+        <v>42636</v>
+      </c>
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="52"/>
+      <c r="A96" s="50"/>
       <c r="B96" s="39">
         <v>26.6</v>
       </c>
@@ -20340,11 +20378,13 @@
       <c r="F96" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G96" s="5"/>
+      <c r="G96" s="10">
+        <v>42636</v>
+      </c>
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
+      <c r="A97" s="50"/>
       <c r="B97" s="39">
         <v>26.7</v>
       </c>
@@ -20360,11 +20400,13 @@
       <c r="F97" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G97" s="5"/>
+      <c r="G97" s="10">
+        <v>42636</v>
+      </c>
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="52"/>
+      <c r="A98" s="50"/>
       <c r="B98" s="39">
         <v>26.8</v>
       </c>
@@ -20380,11 +20422,13 @@
       <c r="F98" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G98" s="5"/>
+      <c r="G98" s="10">
+        <v>42636</v>
+      </c>
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="50"/>
+      <c r="A99" s="51"/>
       <c r="B99" s="39">
         <v>26.9</v>
       </c>
@@ -20400,7 +20444,9 @@
       <c r="F99" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G99" s="3"/>
+      <c r="G99" s="10">
+        <v>42636</v>
+      </c>
       <c r="H99" s="3"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -20446,7 +20492,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="51">
+      <c r="A103" s="49">
         <v>27</v>
       </c>
       <c r="B103" s="5">
@@ -20464,11 +20510,13 @@
       <c r="F103" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G103" s="5"/>
+      <c r="G103" s="10">
+        <v>42636</v>
+      </c>
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="52"/>
+      <c r="A104" s="50"/>
       <c r="B104" s="5">
         <v>27.2</v>
       </c>
@@ -20484,11 +20532,13 @@
       <c r="F104" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G104" s="5"/>
+      <c r="G104" s="10">
+        <v>42636</v>
+      </c>
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="52"/>
+      <c r="A105" s="50"/>
       <c r="B105" s="5">
         <v>27.3</v>
       </c>
@@ -20504,11 +20554,13 @@
       <c r="F105" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G105" s="5"/>
+      <c r="G105" s="10">
+        <v>42636</v>
+      </c>
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="52"/>
+      <c r="A106" s="50"/>
       <c r="B106" s="5">
         <v>27.4</v>
       </c>
@@ -20524,11 +20576,13 @@
       <c r="F106" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G106" s="5"/>
+      <c r="G106" s="10">
+        <v>42636</v>
+      </c>
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="52"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="5">
         <v>27.5</v>
       </c>
@@ -20544,11 +20598,13 @@
       <c r="F107" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G107" s="5"/>
+      <c r="G107" s="10">
+        <v>42636</v>
+      </c>
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="52"/>
+      <c r="A108" s="50"/>
       <c r="B108" s="5">
         <v>27.6</v>
       </c>
@@ -20564,11 +20620,13 @@
       <c r="F108" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G108" s="5"/>
+      <c r="G108" s="10">
+        <v>42636</v>
+      </c>
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="50"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="5">
         <v>27.7</v>
       </c>
@@ -20584,7 +20642,9 @@
       <c r="F109" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G109" s="3"/>
+      <c r="G109" s="10">
+        <v>42636</v>
+      </c>
       <c r="H109" s="3"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -20630,7 +20690,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="62">
+      <c r="A113" s="67">
         <v>4</v>
       </c>
       <c r="B113" s="31">
@@ -20650,7 +20710,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="63"/>
+      <c r="A114" s="70"/>
       <c r="B114" s="31">
         <v>4.2</v>
       </c>
@@ -20668,7 +20728,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="63"/>
+      <c r="A115" s="70"/>
       <c r="B115" s="31">
         <v>4.3</v>
       </c>
@@ -20686,7 +20746,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="63"/>
+      <c r="A116" s="70"/>
       <c r="B116" s="31">
         <v>4.4000000000000004</v>
       </c>
@@ -20704,7 +20764,7 @@
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="63"/>
+      <c r="A117" s="70"/>
       <c r="B117" s="31">
         <v>4.5</v>
       </c>
@@ -20722,7 +20782,7 @@
       <c r="H117" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="63"/>
+      <c r="A118" s="70"/>
       <c r="B118" s="31">
         <v>4.5999999999999996</v>
       </c>
@@ -20740,7 +20800,7 @@
       <c r="H118" s="3"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="63"/>
+      <c r="A119" s="70"/>
       <c r="B119" s="31">
         <v>4.7</v>
       </c>
@@ -20758,7 +20818,7 @@
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="63"/>
+      <c r="A120" s="70"/>
       <c r="B120" s="31">
         <v>4.8</v>
       </c>
@@ -20776,7 +20836,7 @@
       <c r="H120" s="3"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="63"/>
+      <c r="A121" s="70"/>
       <c r="B121" s="31">
         <v>4.9000000000000004</v>
       </c>
@@ -20794,7 +20854,7 @@
       <c r="H121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="64"/>
+      <c r="A122" s="71"/>
       <c r="B122" s="31">
         <v>5</v>
       </c>
@@ -20854,7 +20914,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="51">
+      <c r="A126" s="49">
         <v>30</v>
       </c>
       <c r="B126" s="5">
@@ -20874,7 +20934,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="52"/>
+      <c r="A127" s="50"/>
       <c r="B127" s="5">
         <v>27.2</v>
       </c>
@@ -20892,7 +20952,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="52"/>
+      <c r="A128" s="50"/>
       <c r="B128" s="5">
         <v>27.3</v>
       </c>
@@ -20910,7 +20970,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="52"/>
+      <c r="A129" s="50"/>
       <c r="B129" s="5">
         <v>27.4</v>
       </c>
@@ -20928,7 +20988,7 @@
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="52"/>
+      <c r="A130" s="50"/>
       <c r="B130" s="5">
         <v>27.5</v>
       </c>
@@ -20946,7 +21006,7 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="52"/>
+      <c r="A131" s="50"/>
       <c r="B131" s="5">
         <v>27.6</v>
       </c>
@@ -20964,7 +21024,7 @@
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="50"/>
+      <c r="A132" s="51"/>
       <c r="B132" s="5">
         <v>27.7</v>
       </c>
@@ -21024,7 +21084,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="51">
+      <c r="A136" s="49">
         <v>32</v>
       </c>
       <c r="B136" s="5">
@@ -21044,7 +21104,7 @@
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="52"/>
+      <c r="A137" s="50"/>
       <c r="B137" s="5">
         <v>32.200000000000003</v>
       </c>
@@ -21062,7 +21122,7 @@
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="52"/>
+      <c r="A138" s="50"/>
       <c r="B138" s="5">
         <v>32.299999999999997</v>
       </c>
@@ -21080,7 +21140,7 @@
       <c r="H138" s="3"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="52"/>
+      <c r="A139" s="50"/>
       <c r="B139" s="5">
         <v>32.4</v>
       </c>
@@ -21098,7 +21158,7 @@
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="52"/>
+      <c r="A140" s="50"/>
       <c r="B140" s="5">
         <v>32.5</v>
       </c>
@@ -21116,7 +21176,7 @@
       <c r="H140" s="3"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="52"/>
+      <c r="A141" s="50"/>
       <c r="B141" s="5">
         <v>32.6</v>
       </c>
@@ -21134,7 +21194,7 @@
       <c r="H141" s="3"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="50"/>
+      <c r="A142" s="51"/>
       <c r="B142" s="5">
         <v>32.700000000000003</v>
       </c>
@@ -21153,6 +21213,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="A80:A87"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="G134:H134"/>
     <mergeCell ref="A136:A142"/>
@@ -21169,32 +21255,6 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="G36:H36"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="A80:A87"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:A122"/>
   </mergeCells>
   <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="27" priority="23">

</xml_diff>

<commit_message>
Didnt see we were using the master branch
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="148">
   <si>
     <t>User story: General Website Features</t>
   </si>
@@ -463,6 +463,9 @@
   <si>
     <t>Doesn’t display the planners of the event. Still need to make planners event table.</t>
   </si>
+  <si>
+    <t>Ben(InProgress)</t>
+  </si>
 </sst>
 </file>
 
@@ -737,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -806,18 +809,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -840,15 +843,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -857,11 +863,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,9 +1711,9 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1749,7 +1760,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1783,7 +1794,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>6.2</v>
       </c>
@@ -1808,7 +1819,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>6.3</v>
       </c>
@@ -1833,7 +1844,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>6.4</v>
       </c>
@@ -1858,7 +1869,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>6.5</v>
       </c>
@@ -1881,7 +1892,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="5">
         <v>6.6</v>
       </c>
@@ -1912,17 +1923,17 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="47"/>
       <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="52" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="47"/>
@@ -1956,7 +1967,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="51">
+      <c r="A12" s="49">
         <v>1</v>
       </c>
       <c r="B12" s="17">
@@ -1981,7 +1992,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="17">
         <v>1.2</v>
       </c>
@@ -2004,7 +2015,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="17">
         <v>1.3</v>
       </c>
@@ -2019,7 +2030,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="55">
         <v>1.4</v>
       </c>
@@ -2035,27 +2046,27 @@
       <c r="F15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="53">
         <v>42378</v>
       </c>
       <c r="H15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
       <c r="H16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="16">
         <v>1.5</v>
       </c>
@@ -2089,9 +2100,9 @@
       <c r="A19" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="47"/>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -2130,7 +2141,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51">
+      <c r="A21" s="49">
         <v>11</v>
       </c>
       <c r="B21" s="22">
@@ -2157,7 +2168,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="22">
         <v>11.2</v>
       </c>
@@ -2182,7 +2193,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2204,9 +2215,9 @@
       <c r="A25" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="1" t="s">
         <v>42</v>
@@ -2245,7 +2256,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>12</v>
       </c>
       <c r="B27" s="22">
@@ -2272,7 +2283,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="22">
         <v>12.2</v>
       </c>
@@ -2295,7 +2306,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="22">
         <v>12.3</v>
       </c>
@@ -2338,9 +2349,9 @@
       <c r="A32" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="47"/>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -2379,7 +2390,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="51"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2390,7 +2401,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="52"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2401,7 +2412,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="52"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2412,7 +2423,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="52"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2423,7 +2434,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="52"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2434,7 +2445,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2445,7 +2456,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -10141,15 +10152,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G15:G16"/>
@@ -10161,6 +10163,15 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 A1 F10:G10 A10 F19:G19 A19 F25:G25 A25 F32:G32 A32">
     <cfRule type="notContainsBlanks" dxfId="37" priority="1">
@@ -10197,9 +10208,9 @@
       <c r="A1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="58" t="s">
         <v>1</v>
@@ -10245,7 +10256,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51">
+      <c r="A3" s="49">
         <v>21</v>
       </c>
       <c r="B3" s="5">
@@ -10278,7 +10289,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="5">
         <v>21.2</v>
       </c>
@@ -10302,7 +10313,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="5">
         <v>21.3</v>
       </c>
@@ -10326,7 +10337,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="5">
         <v>21.4</v>
       </c>
@@ -10350,7 +10361,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="5">
         <v>21.5</v>
       </c>
@@ -10372,7 +10383,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="5">
         <v>21.6</v>
       </c>
@@ -10394,7 +10405,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="5">
         <v>21.7</v>
       </c>
@@ -10416,7 +10427,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="5">
         <v>21.8</v>
       </c>
@@ -10440,7 +10451,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="5">
         <v>21.9</v>
       </c>
@@ -10476,9 +10487,9 @@
       <c r="A13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="47"/>
       <c r="F13" s="58" t="s">
         <v>42</v>
@@ -10515,7 +10526,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="51">
+      <c r="A15" s="49">
         <v>20</v>
       </c>
       <c r="B15" s="5">
@@ -10539,7 +10550,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="5">
         <v>20.2</v>
       </c>
@@ -10561,7 +10572,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="5">
         <v>20.3</v>
       </c>
@@ -10585,7 +10596,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -10618,9 +10629,9 @@
       <c r="A20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="47"/>
       <c r="F20" s="58" t="s">
         <v>49</v>
@@ -10657,7 +10668,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51">
+      <c r="A22" s="49">
         <v>5</v>
       </c>
       <c r="B22" s="5">
@@ -10679,7 +10690,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="5">
         <v>5.2</v>
       </c>
@@ -10708,9 +10719,9 @@
       <c r="A25" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="47"/>
       <c r="F25" s="58" t="s">
         <v>40</v>
@@ -10747,7 +10758,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51">
+      <c r="A27" s="49">
         <v>8</v>
       </c>
       <c r="B27" s="5">
@@ -10872,9 +10883,9 @@
       <c r="A33" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="47"/>
       <c r="F33" s="58" t="s">
         <v>70</v>
@@ -10911,7 +10922,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51">
+      <c r="A35" s="49">
         <v>4</v>
       </c>
       <c r="B35" s="5">
@@ -18722,8 +18733,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J119" sqref="J119"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18743,9 +18754,9 @@
       <c r="A1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="47"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
@@ -18788,7 +18799,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="69">
+      <c r="A3" s="62">
         <v>22</v>
       </c>
       <c r="B3" s="31">
@@ -18818,7 +18829,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="69"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="31">
         <v>22.2</v>
       </c>
@@ -18840,7 +18851,7 @@
       <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="69"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="31">
         <v>22.3</v>
       </c>
@@ -18865,9 +18876,9 @@
       <c r="A7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="47"/>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -18904,7 +18915,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="69">
+      <c r="A9" s="62">
         <v>33</v>
       </c>
       <c r="B9" s="31">
@@ -18917,12 +18928,14 @@
         <v>1</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="76" t="s">
+        <v>139</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="33">
         <v>33.200000000000003</v>
       </c>
@@ -18933,12 +18946,14 @@
         <v>1</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="76" t="s">
+        <v>139</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="31">
         <v>33.299999999999997</v>
       </c>
@@ -18949,12 +18964,14 @@
         <v>1</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="76" t="s">
+        <v>139</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="31">
         <v>33.4</v>
       </c>
@@ -18965,12 +18982,14 @@
         <v>1</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
+      <c r="F12" s="76" t="s">
+        <v>139</v>
+      </c>
       <c r="G12" s="18"/>
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="31">
         <v>33.5</v>
       </c>
@@ -18981,7 +19000,9 @@
         <v>0.5</v>
       </c>
       <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="F13" s="76" t="s">
+        <v>139</v>
+      </c>
       <c r="G13" s="31"/>
       <c r="H13" s="34"/>
     </row>
@@ -18989,10 +19010,10 @@
       <c r="A15" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19039,7 +19060,9 @@
         <v>0.5</v>
       </c>
       <c r="E17" s="31"/>
-      <c r="F17" s="28"/>
+      <c r="F17" s="74" t="s">
+        <v>147</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="3"/>
     </row>
@@ -19055,7 +19078,9 @@
         <v>0.5</v>
       </c>
       <c r="E18" s="31"/>
-      <c r="F18" s="28"/>
+      <c r="F18" s="74" t="s">
+        <v>147</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="3"/>
     </row>
@@ -19071,7 +19096,9 @@
         <v>1</v>
       </c>
       <c r="E19" s="31"/>
-      <c r="F19" s="28"/>
+      <c r="F19" s="74" t="s">
+        <v>147</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="3"/>
     </row>
@@ -19087,7 +19114,9 @@
         <v>0.5</v>
       </c>
       <c r="E20" s="31"/>
-      <c r="F20" s="28"/>
+      <c r="F20" s="74" t="s">
+        <v>147</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="3"/>
     </row>
@@ -19103,7 +19132,9 @@
         <v>2</v>
       </c>
       <c r="E21" s="31"/>
-      <c r="F21" s="28"/>
+      <c r="F21" s="74" t="s">
+        <v>147</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="3"/>
     </row>
@@ -19119,7 +19150,9 @@
         <v>1</v>
       </c>
       <c r="E22" s="31"/>
-      <c r="F22" s="28"/>
+      <c r="F22" s="74" t="s">
+        <v>147</v>
+      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="3"/>
     </row>
@@ -19135,7 +19168,9 @@
         <v>0.5</v>
       </c>
       <c r="E23" s="34"/>
-      <c r="F23" s="29"/>
+      <c r="F23" s="74" t="s">
+        <v>147</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
@@ -19147,7 +19182,7 @@
       <c r="C25" s="60"/>
       <c r="D25" s="60"/>
       <c r="E25" s="61"/>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="72" t="s">
         <v>42</v>
       </c>
       <c r="G25" s="46" t="s">
@@ -19182,7 +19217,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="62">
+      <c r="A27" s="67">
         <v>35</v>
       </c>
       <c r="B27" s="5">
@@ -19195,12 +19230,14 @@
         <v>0.5</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="67"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="31">
         <v>35.200000000000003</v>
       </c>
@@ -19211,12 +19248,14 @@
         <v>0.5</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="5">
         <v>35.299999999999997</v>
       </c>
@@ -19227,12 +19266,14 @@
         <v>0.5</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="67"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="31">
         <v>35.4</v>
       </c>
@@ -19243,12 +19284,14 @@
         <v>1</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="F30" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="67"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="5">
         <v>35.5</v>
       </c>
@@ -19259,12 +19302,14 @@
         <v>0.5</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="F31" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="67"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="31">
         <v>35.6</v>
       </c>
@@ -19275,12 +19320,14 @@
         <v>1</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="67"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -19291,12 +19338,14 @@
         <v>1</v>
       </c>
       <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="F33" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="68"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="5">
         <v>35.799999999999997</v>
       </c>
@@ -19307,7 +19356,9 @@
         <v>0.5</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="75" t="s">
+        <v>147</v>
+      </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
@@ -19319,7 +19370,7 @@
       <c r="C36" s="60"/>
       <c r="D36" s="60"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="72" t="s">
         <v>42</v>
       </c>
       <c r="G36" s="46" t="s">
@@ -19354,7 +19405,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="51">
+      <c r="A38" s="49">
         <v>40</v>
       </c>
       <c r="B38" s="5">
@@ -19367,7 +19418,9 @@
         <v>0.5</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="F38" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G38" s="5"/>
       <c r="H38" s="3"/>
     </row>
@@ -19383,7 +19436,9 @@
         <v>2</v>
       </c>
       <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="F39" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G39" s="5"/>
       <c r="H39" s="3"/>
     </row>
@@ -19399,7 +19454,9 @@
         <v>0.5</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
+      <c r="F40" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="3"/>
     </row>
@@ -19415,7 +19472,9 @@
         <v>1</v>
       </c>
       <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
+      <c r="F41" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G41" s="5"/>
       <c r="H41" s="3"/>
     </row>
@@ -19431,7 +19490,9 @@
         <v>1</v>
       </c>
       <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="F42" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="3"/>
     </row>
@@ -19447,7 +19508,9 @@
         <v>1</v>
       </c>
       <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="F43" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G43" s="5"/>
       <c r="H43" s="3"/>
     </row>
@@ -19463,7 +19526,9 @@
         <v>1</v>
       </c>
       <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="F44" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G44" s="5"/>
       <c r="H44" s="3"/>
     </row>
@@ -19479,7 +19544,9 @@
         <v>0.5</v>
       </c>
       <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="F45" s="77" t="s">
+        <v>147</v>
+      </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
@@ -19491,7 +19558,7 @@
       <c r="C47" s="60"/>
       <c r="D47" s="60"/>
       <c r="E47" s="61"/>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="72" t="s">
         <v>70</v>
       </c>
       <c r="G47" s="46" t="s">
@@ -19526,7 +19593,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="51">
+      <c r="A49" s="49">
         <v>23</v>
       </c>
       <c r="B49" s="5">
@@ -19541,7 +19608,7 @@
       <c r="E49" s="5">
         <v>1</v>
       </c>
-      <c r="F49" s="27" t="s">
+      <c r="F49" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G49" s="10">
@@ -19550,7 +19617,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="52"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="5">
         <v>23.2</v>
       </c>
@@ -19563,7 +19630,7 @@
       <c r="E50" s="5">
         <v>1</v>
       </c>
-      <c r="F50" s="27" t="s">
+      <c r="F50" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G50" s="10">
@@ -19572,7 +19639,7 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="52"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="5">
         <v>23.3</v>
       </c>
@@ -19585,7 +19652,7 @@
       <c r="E51" s="5">
         <v>0.5</v>
       </c>
-      <c r="F51" s="27" t="s">
+      <c r="F51" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G51" s="10">
@@ -19594,7 +19661,7 @@
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="52"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="5">
         <v>23.4</v>
       </c>
@@ -19607,7 +19674,7 @@
       <c r="E52" s="5">
         <v>2</v>
       </c>
-      <c r="F52" s="27" t="s">
+      <c r="F52" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G52" s="10">
@@ -19616,7 +19683,7 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="52"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="5">
         <v>23.5</v>
       </c>
@@ -19629,7 +19696,7 @@
       <c r="E53" s="5">
         <v>2</v>
       </c>
-      <c r="F53" s="27" t="s">
+      <c r="F53" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G53" s="10">
@@ -19638,7 +19705,7 @@
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="52"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="5">
         <v>23.6</v>
       </c>
@@ -19651,7 +19718,7 @@
       <c r="E54" s="31">
         <v>1</v>
       </c>
-      <c r="F54" s="27" t="s">
+      <c r="F54" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G54" s="10">
@@ -19660,7 +19727,7 @@
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="52"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="5">
         <v>23.7</v>
       </c>
@@ -19673,7 +19740,7 @@
       <c r="E55" s="5">
         <v>2</v>
       </c>
-      <c r="F55" s="27" t="s">
+      <c r="F55" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G55" s="10">
@@ -19682,7 +19749,7 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="50"/>
+      <c r="A56" s="51"/>
       <c r="B56" s="5">
         <v>23.8</v>
       </c>
@@ -19695,7 +19762,7 @@
       <c r="E56" s="3">
         <v>0.5</v>
       </c>
-      <c r="F56" s="27" t="s">
+      <c r="F56" s="73" t="s">
         <v>17</v>
       </c>
       <c r="G56" s="10">
@@ -19711,7 +19778,7 @@
       <c r="C58" s="60"/>
       <c r="D58" s="60"/>
       <c r="E58" s="61"/>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="72" t="s">
         <v>42</v>
       </c>
       <c r="G58" s="46" t="s">
@@ -19746,7 +19813,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="51">
+      <c r="A60" s="49">
         <v>3</v>
       </c>
       <c r="B60" s="5">
@@ -19759,14 +19826,14 @@
         <v>2</v>
       </c>
       <c r="E60" s="5"/>
-      <c r="F60" s="27" t="s">
-        <v>17</v>
+      <c r="F60" s="73" t="s">
+        <v>139</v>
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="5">
         <v>3.2</v>
       </c>
@@ -19777,14 +19844,14 @@
         <v>0.5</v>
       </c>
       <c r="E61" s="5"/>
-      <c r="F61" s="27" t="s">
-        <v>17</v>
+      <c r="F61" s="73" t="s">
+        <v>139</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="5">
         <v>3.3</v>
       </c>
@@ -19795,14 +19862,14 @@
         <v>1</v>
       </c>
       <c r="E62" s="5"/>
-      <c r="F62" s="27" t="s">
-        <v>17</v>
+      <c r="F62" s="73" t="s">
+        <v>139</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="5">
         <v>3.4</v>
       </c>
@@ -19813,14 +19880,14 @@
         <v>0.5</v>
       </c>
       <c r="E63" s="5"/>
-      <c r="F63" s="27" t="s">
-        <v>17</v>
+      <c r="F63" s="73" t="s">
+        <v>139</v>
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
+      <c r="A64" s="50"/>
       <c r="B64" s="5">
         <v>3.5</v>
       </c>
@@ -19831,14 +19898,14 @@
         <v>2</v>
       </c>
       <c r="E64" s="5"/>
-      <c r="F64" s="27" t="s">
-        <v>17</v>
+      <c r="F64" s="73" t="s">
+        <v>139</v>
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
+      <c r="A65" s="50"/>
       <c r="B65" s="5">
         <v>3.6</v>
       </c>
@@ -19849,14 +19916,14 @@
         <v>1</v>
       </c>
       <c r="E65" s="5"/>
-      <c r="F65" s="27" t="s">
-        <v>17</v>
+      <c r="F65" s="73" t="s">
+        <v>139</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="50"/>
+      <c r="A66" s="51"/>
       <c r="B66" s="5">
         <v>3.7</v>
       </c>
@@ -19867,8 +19934,8 @@
         <v>0.5</v>
       </c>
       <c r="E66" s="3"/>
-      <c r="F66" s="27" t="s">
-        <v>17</v>
+      <c r="F66" s="73" t="s">
+        <v>139</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -19916,7 +19983,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="51">
+      <c r="A70" s="49">
         <v>41</v>
       </c>
       <c r="B70" s="5">
@@ -19936,7 +20003,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="52"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="5">
         <v>41.2</v>
       </c>
@@ -19954,7 +20021,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="52"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="5">
         <v>41.3</v>
       </c>
@@ -19972,7 +20039,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="52"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="5">
         <v>41.4</v>
       </c>
@@ -19990,7 +20057,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="52"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="5">
         <v>41.5</v>
       </c>
@@ -20008,7 +20075,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
+      <c r="A75" s="50"/>
       <c r="B75" s="5">
         <v>41.6</v>
       </c>
@@ -20026,7 +20093,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="50"/>
+      <c r="A76" s="51"/>
       <c r="B76" s="5">
         <v>41.7</v>
       </c>
@@ -20086,7 +20153,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="51">
+      <c r="A80" s="49">
         <v>25</v>
       </c>
       <c r="B80" s="5">
@@ -20110,7 +20177,7 @@
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="52"/>
+      <c r="A81" s="50"/>
       <c r="B81" s="5">
         <v>25.2</v>
       </c>
@@ -20132,7 +20199,7 @@
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="52"/>
+      <c r="A82" s="50"/>
       <c r="B82" s="5">
         <v>25.3</v>
       </c>
@@ -20154,7 +20221,7 @@
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="52"/>
+      <c r="A83" s="50"/>
       <c r="B83" s="5">
         <v>25.4</v>
       </c>
@@ -20176,7 +20243,7 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="52"/>
+      <c r="A84" s="50"/>
       <c r="B84" s="5">
         <v>25.5</v>
       </c>
@@ -20198,7 +20265,7 @@
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="52"/>
+      <c r="A85" s="50"/>
       <c r="B85" s="5">
         <v>25.6</v>
       </c>
@@ -20220,7 +20287,7 @@
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="52"/>
+      <c r="A86" s="50"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -20230,7 +20297,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="50"/>
+      <c r="A87" s="51"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -20282,7 +20349,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="51">
+      <c r="A91" s="49">
         <v>26</v>
       </c>
       <c r="B91" s="39">
@@ -20306,7 +20373,7 @@
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="52"/>
+      <c r="A92" s="50"/>
       <c r="B92" s="39">
         <v>26.2</v>
       </c>
@@ -20328,7 +20395,7 @@
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="52"/>
+      <c r="A93" s="50"/>
       <c r="B93" s="39">
         <v>26.3</v>
       </c>
@@ -20350,7 +20417,7 @@
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="52"/>
+      <c r="A94" s="50"/>
       <c r="B94" s="39">
         <v>26.4</v>
       </c>
@@ -20372,7 +20439,7 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="52"/>
+      <c r="A95" s="50"/>
       <c r="B95" s="39">
         <v>26.5</v>
       </c>
@@ -20394,7 +20461,7 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="52"/>
+      <c r="A96" s="50"/>
       <c r="B96" s="39">
         <v>26.6</v>
       </c>
@@ -20416,7 +20483,7 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
+      <c r="A97" s="50"/>
       <c r="B97" s="39">
         <v>26.7</v>
       </c>
@@ -20438,7 +20505,7 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="52"/>
+      <c r="A98" s="50"/>
       <c r="B98" s="39">
         <v>26.8</v>
       </c>
@@ -20460,7 +20527,7 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="50"/>
+      <c r="A99" s="51"/>
       <c r="B99" s="39">
         <v>26.9</v>
       </c>
@@ -20524,7 +20591,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="51">
+      <c r="A103" s="49">
         <v>27</v>
       </c>
       <c r="B103" s="5">
@@ -20548,7 +20615,7 @@
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="52"/>
+      <c r="A104" s="50"/>
       <c r="B104" s="5">
         <v>27.2</v>
       </c>
@@ -20570,7 +20637,7 @@
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="52"/>
+      <c r="A105" s="50"/>
       <c r="B105" s="5">
         <v>27.3</v>
       </c>
@@ -20592,7 +20659,7 @@
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="52"/>
+      <c r="A106" s="50"/>
       <c r="B106" s="5">
         <v>27.4</v>
       </c>
@@ -20614,7 +20681,7 @@
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="52"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="5">
         <v>27.5</v>
       </c>
@@ -20636,7 +20703,7 @@
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="52"/>
+      <c r="A108" s="50"/>
       <c r="B108" s="5">
         <v>27.6</v>
       </c>
@@ -20658,7 +20725,7 @@
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="50"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="5">
         <v>27.7</v>
       </c>
@@ -20722,7 +20789,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="62">
+      <c r="A113" s="67">
         <v>4</v>
       </c>
       <c r="B113" s="31">
@@ -20746,7 +20813,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="63"/>
+      <c r="A114" s="70"/>
       <c r="B114" s="31">
         <v>4.2</v>
       </c>
@@ -20768,7 +20835,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="63"/>
+      <c r="A115" s="70"/>
       <c r="B115" s="31">
         <v>4.3</v>
       </c>
@@ -20790,7 +20857,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="63"/>
+      <c r="A116" s="70"/>
       <c r="B116" s="31">
         <v>4.4000000000000004</v>
       </c>
@@ -20812,7 +20879,7 @@
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="63"/>
+      <c r="A117" s="70"/>
       <c r="B117" s="31">
         <v>4.5</v>
       </c>
@@ -20834,7 +20901,7 @@
       <c r="H117" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="63"/>
+      <c r="A118" s="70"/>
       <c r="B118" s="31">
         <v>4.5999999999999996</v>
       </c>
@@ -20858,7 +20925,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="63"/>
+      <c r="A119" s="70"/>
       <c r="B119" s="31">
         <v>4.7</v>
       </c>
@@ -20880,7 +20947,7 @@
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="63"/>
+      <c r="A120" s="70"/>
       <c r="B120" s="31">
         <v>4.8</v>
       </c>
@@ -20900,7 +20967,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="63"/>
+      <c r="A121" s="70"/>
       <c r="B121" s="31">
         <v>4.9000000000000004</v>
       </c>
@@ -20924,7 +20991,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="64"/>
+      <c r="A122" s="71"/>
       <c r="B122" s="32" t="s">
         <v>141</v>
       </c>
@@ -20990,7 +21057,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="51">
+      <c r="A126" s="49">
         <v>30</v>
       </c>
       <c r="B126" s="5">
@@ -21010,7 +21077,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="52"/>
+      <c r="A127" s="50"/>
       <c r="B127" s="5">
         <v>27.2</v>
       </c>
@@ -21028,7 +21095,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="52"/>
+      <c r="A128" s="50"/>
       <c r="B128" s="5">
         <v>27.3</v>
       </c>
@@ -21046,7 +21113,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="52"/>
+      <c r="A129" s="50"/>
       <c r="B129" s="5">
         <v>27.4</v>
       </c>
@@ -21064,7 +21131,7 @@
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="52"/>
+      <c r="A130" s="50"/>
       <c r="B130" s="5">
         <v>27.5</v>
       </c>
@@ -21082,7 +21149,7 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="52"/>
+      <c r="A131" s="50"/>
       <c r="B131" s="5">
         <v>27.6</v>
       </c>
@@ -21100,7 +21167,7 @@
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="50"/>
+      <c r="A132" s="51"/>
       <c r="B132" s="5">
         <v>27.7</v>
       </c>
@@ -21160,7 +21227,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="51">
+      <c r="A136" s="49">
         <v>32</v>
       </c>
       <c r="B136" s="5">
@@ -21182,7 +21249,7 @@
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="52"/>
+      <c r="A137" s="50"/>
       <c r="B137" s="5">
         <v>32.200000000000003</v>
       </c>
@@ -21202,7 +21269,7 @@
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="52"/>
+      <c r="A138" s="50"/>
       <c r="B138" s="5">
         <v>32.299999999999997</v>
       </c>
@@ -21222,7 +21289,7 @@
       <c r="H138" s="3"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="52"/>
+      <c r="A139" s="50"/>
       <c r="B139" s="5">
         <v>32.4</v>
       </c>
@@ -21242,7 +21309,7 @@
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="52"/>
+      <c r="A140" s="50"/>
       <c r="B140" s="5">
         <v>32.5</v>
       </c>
@@ -21264,7 +21331,7 @@
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="52"/>
+      <c r="A141" s="50"/>
       <c r="B141" s="5">
         <v>32.6</v>
       </c>
@@ -21284,7 +21351,7 @@
       <c r="H141" s="3"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="50"/>
+      <c r="A142" s="51"/>
       <c r="B142" s="5">
         <v>32.700000000000003</v>
       </c>
@@ -21305,6 +21372,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="A80:A87"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="G134:H134"/>
     <mergeCell ref="A136:A142"/>
@@ -21321,32 +21414,6 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="G36:H36"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="A80:A87"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:A122"/>
   </mergeCells>
   <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="27" priority="23">

</xml_diff>

<commit_message>
Im doing the volunteers list now
So that we can have as many of these done by monday.
If you need help in your assigned task, please just ask.
</commit_message>
<xml_diff>
--- a/Task Assignment Sheet.xlsx
+++ b/Task Assignment Sheet.xlsx
@@ -817,18 +817,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -851,15 +851,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -868,11 +871,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1711,9 +1711,9 @@
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="53"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1760,7 +1760,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57">
+      <c r="A3" s="55">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1794,7 +1794,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="5">
         <v>6.2</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="5">
         <v>6.3</v>
       </c>
@@ -1844,7 +1844,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="5">
         <v>6.4</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="5">
         <v>6.5</v>
       </c>
@@ -1892,7 +1892,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="56"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="5">
         <v>6.6</v>
       </c>
@@ -1923,17 +1923,17 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
       <c r="E10" s="53"/>
       <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="58" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="53"/>
@@ -1967,7 +1967,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57">
+      <c r="A12" s="55">
         <v>1</v>
       </c>
       <c r="B12" s="17">
@@ -1992,7 +1992,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="58"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="17">
         <v>1.2</v>
       </c>
@@ -2015,7 +2015,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="58"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="17">
         <v>1.3</v>
       </c>
@@ -2030,7 +2030,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="58"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="61">
         <v>1.4</v>
       </c>
@@ -2046,27 +2046,27 @@
       <c r="F15" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="55">
+      <c r="G15" s="59">
         <v>42378</v>
       </c>
       <c r="H15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="58"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="56"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="16">
         <v>1.5</v>
       </c>
@@ -2100,9 +2100,9 @@
       <c r="A19" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="53"/>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -2141,7 +2141,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57">
+      <c r="A21" s="55">
         <v>11</v>
       </c>
       <c r="B21" s="22">
@@ -2168,7 +2168,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="22">
         <v>11.2</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="56"/>
+      <c r="A23" s="57"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2215,9 +2215,9 @@
       <c r="A25" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="53"/>
       <c r="F25" s="1" t="s">
         <v>42</v>
@@ -2256,7 +2256,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="57">
+      <c r="A27" s="55">
         <v>12</v>
       </c>
       <c r="B27" s="22">
@@ -2283,7 +2283,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="22">
         <v>12.2</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="22">
         <v>12.3</v>
       </c>
@@ -2349,9 +2349,9 @@
       <c r="A32" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
       <c r="E32" s="53"/>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -2390,7 +2390,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="57"/>
+      <c r="A34" s="55"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2401,7 +2401,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="58"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2412,7 +2412,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="58"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2423,7 +2423,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="58"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2434,7 +2434,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="58"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2445,7 +2445,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="58"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2456,7 +2456,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="56"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -10152,15 +10152,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G15:G16"/>
@@ -10172,6 +10163,15 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:G1 A1 F10:G10 A10 F19:G19 A19 F25:G25 A25 F32:G32 A32">
     <cfRule type="notContainsBlanks" dxfId="37" priority="1">
@@ -10208,9 +10208,9 @@
       <c r="A1" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="53"/>
       <c r="F1" s="64" t="s">
         <v>1</v>
@@ -10256,7 +10256,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57">
+      <c r="A3" s="55">
         <v>21</v>
       </c>
       <c r="B3" s="5">
@@ -10289,7 +10289,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="5">
         <v>21.2</v>
       </c>
@@ -10313,7 +10313,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="5">
         <v>21.3</v>
       </c>
@@ -10337,7 +10337,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="5">
         <v>21.4</v>
       </c>
@@ -10361,7 +10361,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="5">
         <v>21.5</v>
       </c>
@@ -10383,7 +10383,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="58"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="5">
         <v>21.6</v>
       </c>
@@ -10405,7 +10405,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="58"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="5">
         <v>21.7</v>
       </c>
@@ -10427,7 +10427,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="58"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="5">
         <v>21.8</v>
       </c>
@@ -10451,7 +10451,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="56"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="5">
         <v>21.9</v>
       </c>
@@ -10487,9 +10487,9 @@
       <c r="A13" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="53"/>
       <c r="F13" s="64" t="s">
         <v>42</v>
@@ -10526,7 +10526,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57">
+      <c r="A15" s="55">
         <v>20</v>
       </c>
       <c r="B15" s="5">
@@ -10550,7 +10550,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="58"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="5">
         <v>20.2</v>
       </c>
@@ -10572,7 +10572,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="58"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="5">
         <v>20.3</v>
       </c>
@@ -10596,7 +10596,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="56"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -10629,9 +10629,9 @@
       <c r="A20" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="53"/>
       <c r="F20" s="64" t="s">
         <v>49</v>
@@ -10668,7 +10668,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="57">
+      <c r="A22" s="55">
         <v>5</v>
       </c>
       <c r="B22" s="5">
@@ -10690,7 +10690,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="56"/>
+      <c r="A23" s="57"/>
       <c r="B23" s="5">
         <v>5.2</v>
       </c>
@@ -10719,9 +10719,9 @@
       <c r="A25" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="53"/>
       <c r="F25" s="64" t="s">
         <v>40</v>
@@ -10758,7 +10758,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="57">
+      <c r="A27" s="55">
         <v>8</v>
       </c>
       <c r="B27" s="5">
@@ -10883,9 +10883,9 @@
       <c r="A33" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="53"/>
       <c r="F33" s="64" t="s">
         <v>70</v>
@@ -10922,7 +10922,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57">
+      <c r="A35" s="55">
         <v>4</v>
       </c>
       <c r="B35" s="5">
@@ -18733,8 +18733,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N134" sqref="N134"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18754,9 +18754,9 @@
       <c r="A1" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="53"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
@@ -18799,7 +18799,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="75">
+      <c r="A3" s="68">
         <v>22</v>
       </c>
       <c r="B3" s="31">
@@ -18829,7 +18829,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="75"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="31">
         <v>22.2</v>
       </c>
@@ -18851,7 +18851,7 @@
       <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="75"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="31">
         <v>22.3</v>
       </c>
@@ -18876,9 +18876,9 @@
       <c r="A7" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="53"/>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -18915,7 +18915,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="75">
+      <c r="A9" s="68">
         <v>33</v>
       </c>
       <c r="B9" s="31">
@@ -18935,7 +18935,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="75"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="33">
         <v>33.200000000000003</v>
       </c>
@@ -18953,7 +18953,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="75"/>
+      <c r="A11" s="68"/>
       <c r="B11" s="31">
         <v>33.299999999999997</v>
       </c>
@@ -18971,7 +18971,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="75"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="31">
         <v>33.4</v>
       </c>
@@ -18989,7 +18989,7 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="75"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="31">
         <v>33.5</v>
       </c>
@@ -19010,10 +19010,10 @@
       <c r="A15" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="77"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19217,7 +19217,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="68">
+      <c r="A27" s="73">
         <v>35</v>
       </c>
       <c r="B27" s="5">
@@ -19237,7 +19237,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="73"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="31">
         <v>35.200000000000003</v>
       </c>
@@ -19255,7 +19255,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="73"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="5">
         <v>35.299999999999997</v>
       </c>
@@ -19273,7 +19273,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="73"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="31">
         <v>35.4</v>
       </c>
@@ -19291,7 +19291,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="73"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="5">
         <v>35.5</v>
       </c>
@@ -19309,7 +19309,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="73"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="31">
         <v>35.6</v>
       </c>
@@ -19327,7 +19327,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="73"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -19345,7 +19345,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="74"/>
+      <c r="A34" s="75"/>
       <c r="B34" s="5">
         <v>35.799999999999997</v>
       </c>
@@ -19405,7 +19405,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="57">
+      <c r="A38" s="55">
         <v>40</v>
       </c>
       <c r="B38" s="5">
@@ -19593,7 +19593,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="57">
+      <c r="A49" s="55">
         <v>23</v>
       </c>
       <c r="B49" s="5">
@@ -19617,7 +19617,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="58"/>
+      <c r="A50" s="56"/>
       <c r="B50" s="5">
         <v>23.2</v>
       </c>
@@ -19639,7 +19639,7 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="58"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="5">
         <v>23.3</v>
       </c>
@@ -19661,7 +19661,7 @@
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="58"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="5">
         <v>23.4</v>
       </c>
@@ -19683,7 +19683,7 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="58"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="5">
         <v>23.5</v>
       </c>
@@ -19705,7 +19705,7 @@
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="58"/>
+      <c r="A54" s="56"/>
       <c r="B54" s="5">
         <v>23.6</v>
       </c>
@@ -19727,7 +19727,7 @@
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="58"/>
+      <c r="A55" s="56"/>
       <c r="B55" s="5">
         <v>23.7</v>
       </c>
@@ -19749,7 +19749,7 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="56"/>
+      <c r="A56" s="57"/>
       <c r="B56" s="5">
         <v>23.8</v>
       </c>
@@ -19813,7 +19813,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="57">
+      <c r="A60" s="55">
         <v>3</v>
       </c>
       <c r="B60" s="5">
@@ -19826,14 +19826,14 @@
         <v>2</v>
       </c>
       <c r="E60" s="5"/>
-      <c r="F60" s="47" t="s">
-        <v>139</v>
+      <c r="F60" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="58"/>
+      <c r="A61" s="56"/>
       <c r="B61" s="5">
         <v>3.2</v>
       </c>
@@ -19844,14 +19844,14 @@
         <v>0.5</v>
       </c>
       <c r="E61" s="5"/>
-      <c r="F61" s="47" t="s">
-        <v>139</v>
+      <c r="F61" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="58"/>
+      <c r="A62" s="56"/>
       <c r="B62" s="5">
         <v>3.3</v>
       </c>
@@ -19862,14 +19862,14 @@
         <v>1</v>
       </c>
       <c r="E62" s="5"/>
-      <c r="F62" s="47" t="s">
-        <v>139</v>
+      <c r="F62" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="58"/>
+      <c r="A63" s="56"/>
       <c r="B63" s="5">
         <v>3.4</v>
       </c>
@@ -19880,14 +19880,14 @@
         <v>0.5</v>
       </c>
       <c r="E63" s="5"/>
-      <c r="F63" s="47" t="s">
-        <v>139</v>
+      <c r="F63" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="58"/>
+      <c r="A64" s="56"/>
       <c r="B64" s="5">
         <v>3.5</v>
       </c>
@@ -19898,14 +19898,14 @@
         <v>2</v>
       </c>
       <c r="E64" s="5"/>
-      <c r="F64" s="47" t="s">
-        <v>139</v>
+      <c r="F64" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="58"/>
+      <c r="A65" s="56"/>
       <c r="B65" s="5">
         <v>3.6</v>
       </c>
@@ -19916,14 +19916,14 @@
         <v>1</v>
       </c>
       <c r="E65" s="5"/>
-      <c r="F65" s="47" t="s">
-        <v>139</v>
+      <c r="F65" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="56"/>
+      <c r="A66" s="57"/>
       <c r="B66" s="5">
         <v>3.7</v>
       </c>
@@ -19934,8 +19934,8 @@
         <v>0.5</v>
       </c>
       <c r="E66" s="3"/>
-      <c r="F66" s="47" t="s">
-        <v>139</v>
+      <c r="F66" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -19983,7 +19983,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="57">
+      <c r="A70" s="55">
         <v>41</v>
       </c>
       <c r="B70" s="5">
@@ -20003,7 +20003,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="58"/>
+      <c r="A71" s="56"/>
       <c r="B71" s="5">
         <v>41.2</v>
       </c>
@@ -20021,7 +20021,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="58"/>
+      <c r="A72" s="56"/>
       <c r="B72" s="5">
         <v>41.3</v>
       </c>
@@ -20039,7 +20039,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="58"/>
+      <c r="A73" s="56"/>
       <c r="B73" s="5">
         <v>41.4</v>
       </c>
@@ -20057,7 +20057,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="58"/>
+      <c r="A74" s="56"/>
       <c r="B74" s="5">
         <v>41.5</v>
       </c>
@@ -20075,7 +20075,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="58"/>
+      <c r="A75" s="56"/>
       <c r="B75" s="5">
         <v>41.6</v>
       </c>
@@ -20093,7 +20093,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="56"/>
+      <c r="A76" s="57"/>
       <c r="B76" s="5">
         <v>41.7</v>
       </c>
@@ -20153,7 +20153,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="57">
+      <c r="A80" s="55">
         <v>25</v>
       </c>
       <c r="B80" s="5">
@@ -20177,7 +20177,7 @@
       <c r="H80" s="3"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="58"/>
+      <c r="A81" s="56"/>
       <c r="B81" s="5">
         <v>25.2</v>
       </c>
@@ -20199,7 +20199,7 @@
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="58"/>
+      <c r="A82" s="56"/>
       <c r="B82" s="5">
         <v>25.3</v>
       </c>
@@ -20221,7 +20221,7 @@
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="58"/>
+      <c r="A83" s="56"/>
       <c r="B83" s="5">
         <v>25.4</v>
       </c>
@@ -20243,7 +20243,7 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="58"/>
+      <c r="A84" s="56"/>
       <c r="B84" s="5">
         <v>25.5</v>
       </c>
@@ -20265,7 +20265,7 @@
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="58"/>
+      <c r="A85" s="56"/>
       <c r="B85" s="5">
         <v>25.6</v>
       </c>
@@ -20287,7 +20287,7 @@
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="58"/>
+      <c r="A86" s="56"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -20297,7 +20297,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="56"/>
+      <c r="A87" s="57"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -20349,7 +20349,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="57">
+      <c r="A91" s="55">
         <v>26</v>
       </c>
       <c r="B91" s="39">
@@ -20373,7 +20373,7 @@
       <c r="H91" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="58"/>
+      <c r="A92" s="56"/>
       <c r="B92" s="39">
         <v>26.2</v>
       </c>
@@ -20395,7 +20395,7 @@
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="58"/>
+      <c r="A93" s="56"/>
       <c r="B93" s="39">
         <v>26.3</v>
       </c>
@@ -20417,7 +20417,7 @@
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="58"/>
+      <c r="A94" s="56"/>
       <c r="B94" s="39">
         <v>26.4</v>
       </c>
@@ -20439,7 +20439,7 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="58"/>
+      <c r="A95" s="56"/>
       <c r="B95" s="39">
         <v>26.5</v>
       </c>
@@ -20461,7 +20461,7 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="58"/>
+      <c r="A96" s="56"/>
       <c r="B96" s="39">
         <v>26.6</v>
       </c>
@@ -20483,7 +20483,7 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="58"/>
+      <c r="A97" s="56"/>
       <c r="B97" s="39">
         <v>26.7</v>
       </c>
@@ -20505,7 +20505,7 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="58"/>
+      <c r="A98" s="56"/>
       <c r="B98" s="39">
         <v>26.8</v>
       </c>
@@ -20527,7 +20527,7 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="56"/>
+      <c r="A99" s="57"/>
       <c r="B99" s="39">
         <v>26.9</v>
       </c>
@@ -20591,7 +20591,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="57">
+      <c r="A103" s="55">
         <v>27</v>
       </c>
       <c r="B103" s="5">
@@ -20615,7 +20615,7 @@
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="58"/>
+      <c r="A104" s="56"/>
       <c r="B104" s="5">
         <v>27.2</v>
       </c>
@@ -20637,7 +20637,7 @@
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="58"/>
+      <c r="A105" s="56"/>
       <c r="B105" s="5">
         <v>27.3</v>
       </c>
@@ -20659,7 +20659,7 @@
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="58"/>
+      <c r="A106" s="56"/>
       <c r="B106" s="5">
         <v>27.4</v>
       </c>
@@ -20681,7 +20681,7 @@
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="58"/>
+      <c r="A107" s="56"/>
       <c r="B107" s="5">
         <v>27.5</v>
       </c>
@@ -20703,7 +20703,7 @@
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="58"/>
+      <c r="A108" s="56"/>
       <c r="B108" s="5">
         <v>27.6</v>
       </c>
@@ -20725,7 +20725,7 @@
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="56"/>
+      <c r="A109" s="57"/>
       <c r="B109" s="5">
         <v>27.7</v>
       </c>
@@ -20789,7 +20789,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="68">
+      <c r="A113" s="73">
         <v>4</v>
       </c>
       <c r="B113" s="31">
@@ -20813,7 +20813,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="69"/>
+      <c r="A114" s="76"/>
       <c r="B114" s="31">
         <v>4.2</v>
       </c>
@@ -20835,7 +20835,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="69"/>
+      <c r="A115" s="76"/>
       <c r="B115" s="31">
         <v>4.3</v>
       </c>
@@ -20857,7 +20857,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="69"/>
+      <c r="A116" s="76"/>
       <c r="B116" s="31">
         <v>4.4000000000000004</v>
       </c>
@@ -20879,7 +20879,7 @@
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="69"/>
+      <c r="A117" s="76"/>
       <c r="B117" s="31">
         <v>4.5</v>
       </c>
@@ -20901,7 +20901,7 @@
       <c r="H117" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="69"/>
+      <c r="A118" s="76"/>
       <c r="B118" s="31">
         <v>4.5999999999999996</v>
       </c>
@@ -20925,7 +20925,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="69"/>
+      <c r="A119" s="76"/>
       <c r="B119" s="31">
         <v>4.7</v>
       </c>
@@ -20947,7 +20947,7 @@
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="69"/>
+      <c r="A120" s="76"/>
       <c r="B120" s="31">
         <v>4.8</v>
       </c>
@@ -20967,7 +20967,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="69"/>
+      <c r="A121" s="76"/>
       <c r="B121" s="31">
         <v>4.9000000000000004</v>
       </c>
@@ -20991,7 +20991,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="70"/>
+      <c r="A122" s="77"/>
       <c r="B122" s="32" t="s">
         <v>141</v>
       </c>
@@ -21057,7 +21057,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="57">
+      <c r="A126" s="55">
         <v>30</v>
       </c>
       <c r="B126" s="5">
@@ -21077,7 +21077,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="58"/>
+      <c r="A127" s="56"/>
       <c r="B127" s="5">
         <v>27.2</v>
       </c>
@@ -21095,7 +21095,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="58"/>
+      <c r="A128" s="56"/>
       <c r="B128" s="5">
         <v>27.3</v>
       </c>
@@ -21113,7 +21113,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="58"/>
+      <c r="A129" s="56"/>
       <c r="B129" s="5">
         <v>27.4</v>
       </c>
@@ -21131,7 +21131,7 @@
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="58"/>
+      <c r="A130" s="56"/>
       <c r="B130" s="5">
         <v>27.5</v>
       </c>
@@ -21149,7 +21149,7 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="58"/>
+      <c r="A131" s="56"/>
       <c r="B131" s="5">
         <v>27.6</v>
       </c>
@@ -21167,7 +21167,7 @@
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="56"/>
+      <c r="A132" s="57"/>
       <c r="B132" s="5">
         <v>27.7</v>
       </c>
@@ -21227,7 +21227,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="57">
+      <c r="A136" s="55">
         <v>32</v>
       </c>
       <c r="B136" s="5">
@@ -21251,7 +21251,7 @@
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="58"/>
+      <c r="A137" s="56"/>
       <c r="B137" s="5">
         <v>32.200000000000003</v>
       </c>
@@ -21273,7 +21273,7 @@
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="58"/>
+      <c r="A138" s="56"/>
       <c r="B138" s="5">
         <v>32.299999999999997</v>
       </c>
@@ -21295,7 +21295,7 @@
       <c r="H138" s="3"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="58"/>
+      <c r="A139" s="56"/>
       <c r="B139" s="5">
         <v>32.4</v>
       </c>
@@ -21317,7 +21317,7 @@
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="58"/>
+      <c r="A140" s="56"/>
       <c r="B140" s="5">
         <v>32.5</v>
       </c>
@@ -21341,7 +21341,7 @@
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="58"/>
+      <c r="A141" s="56"/>
       <c r="B141" s="5">
         <v>32.6</v>
       </c>
@@ -21363,7 +21363,7 @@
       <c r="H141" s="3"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="56"/>
+      <c r="A142" s="57"/>
       <c r="B142" s="5">
         <v>32.700000000000003</v>
       </c>
@@ -21386,6 +21386,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="A80:A87"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="G134:H134"/>
     <mergeCell ref="A136:A142"/>
@@ -21402,32 +21428,6 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="G36:H36"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="A80:A87"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:A122"/>
   </mergeCells>
   <conditionalFormatting sqref="A36">
     <cfRule type="notContainsBlanks" dxfId="27" priority="23">

</xml_diff>